<commit_message>
Made changes to modular FrEDI data processing
Made changes to modular FrEDI data processing
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16098DB-DD22-4DBA-85C6-8ABEBA2930CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F05D944-288B-4983-9F50-62662DD09A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5595" yWindow="-27450" windowWidth="18945" windowHeight="24630" tabRatio="764" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="loc_coConstants">co_constants[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coImpactTypes">co_impactTypes[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coImpactYears">co_impactYears[[#Headers],[row_id]]</definedName>
-    <definedName name="loc_coInputScenarioInfo">co_inputScenarioInfo[[#Headers],[row_id]]</definedName>
+    <definedName name="loc_coInputScenarioInfo">co_inputInfo[[#Headers],[row_id]]</definedName>
     <definedName name="loc_colorLegend">controlTables!$C$16</definedName>
     <definedName name="loc_coModels">co_models[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coModelTypes">co_modelTypes[[#Headers],[row_id]]</definedName>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="607">
   <si>
     <t>CanESM2</t>
   </si>
@@ -2126,6 +2126,9 @@
   </si>
   <si>
     <t>region_id</t>
+  </si>
+  <si>
+    <t>co_inputInfo</t>
   </si>
 </sst>
 </file>
@@ -3265,20 +3268,6 @@
     <cellStyle name="z A Column text" xfId="12" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
   </cellStyles>
   <dxfs count="198">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5568,6 +5557,20 @@
         <name val="Calibri"/>
         <family val="2"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -7600,62 +7603,62 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B174:J208" totalsRowShown="0" headerRowDxfId="88" dataDxfId="87">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B174:J208" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
   <autoFilter ref="B174:J208" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B175:J203">
     <sortCondition ref="E175:E203"/>
     <sortCondition ref="C175:C203"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="86">
+    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="85">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarName" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{11586BC8-9866-411F-AFB1-B54CDBE58BC8}" name="scalarLabel" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{59273865-10D7-4E58-A34B-98B12FD27367}" name="scalarType" dataDxfId="83"/>
-    <tableColumn id="6" xr3:uid="{44722630-DE32-4127-9D36-E5716D7B6FB1}" name="constant_or_dynamic" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{06B55EB3-A830-4A09-BCEF-732F610DB775}" name="national_or_regional" dataDxfId="81"/>
-    <tableColumn id="12" xr3:uid="{DA5FA732-C673-49CC-B393-EEDF239C5944}" name="valueYear" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{072DFA28-3A99-48D9-9F87-0B9663CC8EBE}" name="dataType" dataDxfId="79"/>
-    <tableColumn id="8" xr3:uid="{083C27B7-8723-4638-8D25-C880E916AEB0}" name="notes" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarName" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{11586BC8-9866-411F-AFB1-B54CDBE58BC8}" name="scalarLabel" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{59273865-10D7-4E58-A34B-98B12FD27367}" name="scalarType" dataDxfId="82"/>
+    <tableColumn id="6" xr3:uid="{44722630-DE32-4127-9D36-E5716D7B6FB1}" name="constant_or_dynamic" dataDxfId="81"/>
+    <tableColumn id="7" xr3:uid="{06B55EB3-A830-4A09-BCEF-732F610DB775}" name="national_or_regional" dataDxfId="80"/>
+    <tableColumn id="12" xr3:uid="{DA5FA732-C673-49CC-B393-EEDF239C5944}" name="valueYear" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{072DFA28-3A99-48D9-9F87-0B9663CC8EBE}" name="dataType" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{083C27B7-8723-4638-8D25-C880E916AEB0}" name="notes" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B221:D224" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B221:D224" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D7815580-A46D-4035-AF95-6DFB7EDC1C86}" name="row_id" dataDxfId="75">
+    <tableColumn id="1" xr3:uid="{D7815580-A46D-4035-AF95-6DFB7EDC1C86}" name="row_id" dataDxfId="74">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7CEFD3F0-E79C-4BEE-B910-4D600E302386}" name="constant" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{DB7DDBBB-C95A-4211-819C-B05A5C2E7319}" name="value" dataDxfId="73" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{7CEFD3F0-E79C-4BEE-B910-4D600E302386}" name="constant" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{DB7DDBBB-C95A-4211-819C-B05A5C2E7319}" name="value" dataDxfId="72" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B80:I122" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B80:I122" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="B80:I122" xr:uid="{2B645CB4-F641-4C38-A983-F38F00FA7B52}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B81:I122">
     <sortCondition ref="C81:C122"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="70" totalsRowDxfId="69">
+    <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="69" totalsRowDxfId="68">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{11CBE921-72AF-48C1-82DE-27D30284B810}" name="sector_id" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{1A31D87B-CDD5-4D8C-A4C9-8892B2B2C1E8}" name="variant_label" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{BD980D22-60C8-4EA5-878C-1F6646D73814}" name="variant_id" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="7" xr3:uid="{77C8D2EF-4466-45BD-90C6-9DB11F371760}" name="sectorprimary" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{677E6396-DB82-43C2-B1C8-9CF8A385BC06}" name="includeaggregate" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="19" xr3:uid="{C16D6C81-A98D-4F3D-B812-6AFD7158219C}" name="damageAdjName" dataDxfId="58" totalsRowDxfId="57">
+    <tableColumn id="18" xr3:uid="{11CBE921-72AF-48C1-82DE-27D30284B810}" name="sector_id" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{1A31D87B-CDD5-4D8C-A4C9-8892B2B2C1E8}" name="variant_label" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{BD980D22-60C8-4EA5-878C-1F6646D73814}" name="variant_id" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{77C8D2EF-4466-45BD-90C6-9DB11F371760}" name="sectorprimary" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{677E6396-DB82-43C2-B1C8-9CF8A385BC06}" name="includeaggregate" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="19" xr3:uid="{C16D6C81-A98D-4F3D-B812-6AFD7158219C}" name="damageAdjName" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( co_variants[[#This Row],[sector_id]] = "Roads","_" &amp; co_variants[[#This Row],[variant_id]], "" )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DBDAE92A-E63D-41B7-BD88-AE325DF1F4FE}" name="hasImpacts" dataDxfId="56">
+    <tableColumn id="8" xr3:uid="{DBDAE92A-E63D-41B7-BD88-AE325DF1F4FE}" name="hasImpacts" dataDxfId="55">
       <calculatedColumnFormula array="1" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt; 1 )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7664,68 +7667,68 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B213:E216" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B213:E216" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="52">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierDescription" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierDescription" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputScenarioInfo" displayName="co_inputScenarioInfo" ref="B263:J267" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B263:J267" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="47">
-      <calculatedColumnFormula xml:space="preserve"> ROW( co_inputScenarioInfo[[#This Row],[row_id]] ) - ROW( co_inputScenarioInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="46">
+      <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{98CB64F8-23F0-4402-9CE1-03695A07036B}" name="inputDesc" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="41">
-      <calculatedColumnFormula xml:space="preserve"> IF( ISNA( MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{98CB64F8-23F0-4402-9CE1-03695A07036B}" name="inputDesc" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="40">
+      <calculatedColumnFormula xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="region" dataDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="region" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B284:F333" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B284:F333" totalsRowShown="0" headerRowDxfId="37">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="37">
+    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="36">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{F4F2D0D4-82EF-41DF-B43B-E23CB36CF080}" name="region" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{F4F2D0D4-82EF-41DF-B43B-E23CB36CF080}" name="region" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B230:I232" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B230:I232" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{39608CCF-EBE2-4EFA-BA66-990DD890C7D3}" name="row_id" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{39608CCF-EBE2-4EFA-BA66-990DD890C7D3}" name="row_id" dataDxfId="29">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{24491F20-89B9-4A6B-A87E-CDB3D398E1DA}" name="sector" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{60DDD337-313C-431F-83CE-788A259B2B14}" name="physScalarName" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{AB34CD40-6627-470D-9B2F-2360E9A41A63}" name="econMultiplierName" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{774FF8C9-540D-4647-BB5C-0F27D92917EB}" name="c1" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{6D77C177-ACD8-474A-9CEF-58627396E0D5}" name="exp0" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{45D5B794-1A45-47DA-8A77-45C881CC1B29}" name="c2" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{07C4CFF2-DEE6-4176-813C-12CE016805C3}" name="refYear" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{24491F20-89B9-4A6B-A87E-CDB3D398E1DA}" name="sector" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{60DDD337-313C-431F-83CE-788A259B2B14}" name="physScalarName" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{AB34CD40-6627-470D-9B2F-2360E9A41A63}" name="econMultiplierName" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{774FF8C9-540D-4647-BB5C-0F27D92917EB}" name="c1" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{6D77C177-ACD8-474A-9CEF-58627396E0D5}" name="exp0" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{45D5B794-1A45-47DA-8A77-45C881CC1B29}" name="c2" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{07C4CFF2-DEE6-4176-813C-12CE016805C3}" name="refYear" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7735,10 +7738,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}" name="Readme_adaptations" displayName="Readme_adaptations" ref="B9:E15" totalsRowShown="0">
   <autoFilter ref="B9:E15" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="21">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_adaptations[[#This Row],[row_id]] ) - ROW( Readme_adaptations[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{13712644-0D89-49D5-9571-32BD03BF1BD3}" name="adapt_id"/>
     <tableColumn id="3" xr3:uid="{B89736B7-3040-4F82-B2CC-EB15F47F50B3}" name="adapt_label"/>
   </tableColumns>
@@ -7747,16 +7750,16 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="B3:F5" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="17">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_sectors[[#This Row],[row_id]] ) - ROW( Readme_sectors[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7766,17 +7769,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}" name="slr_cm" displayName="slr_cm" ref="A1:I102" totalsRowShown="0">
   <autoFilter ref="A1:I102" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="13">
+    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="12">
       <calculatedColumnFormula xml:space="preserve"> ROW( slr_cm[[#This Row],[row_id]] ) - ROW( slr_cm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7918,7 +7921,7 @@
       <calculatedColumnFormula xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{56B07D04-3458-4687-B04E-181849066DB3}" name="region_label" dataDxfId="126"/>
-    <tableColumn id="5" xr3:uid="{FFA64F27-24E0-4D92-8E8A-6A4675CEB856}" name="region_id" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{FFA64F27-24E0-4D92-8E8A-6A4675CEB856}" name="region_id" dataDxfId="125">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7927,16 +7930,16 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B244:G258" totalsRowShown="0" headerRowDxfId="125" dataDxfId="124">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B244:G258" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="123">
+    <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="122">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A209304D-718C-45BB-922A-A83B3EC89858}" name="model_id" dataDxfId="122"/>
-    <tableColumn id="5" xr3:uid="{CBC70E09-D146-4CF4-911F-60EB221755C0}" name="maxUnitValue" dataDxfId="121"/>
-    <tableColumn id="20" xr3:uid="{A1F83970-3B0E-4464-8376-1B37DBE20974}" name="modelType" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{F9DE0808-4FD0-4FB6-9363-B580ED760D5C}" name="model_label" dataDxfId="119"/>
-    <tableColumn id="6" xr3:uid="{2D75E915-5C37-41D0-8D80-E36A15696E43}" name="model_underscore" dataDxfId="118">
+    <tableColumn id="2" xr3:uid="{A209304D-718C-45BB-922A-A83B3EC89858}" name="model_id" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{CBC70E09-D146-4CF4-911F-60EB221755C0}" name="maxUnitValue" dataDxfId="120"/>
+    <tableColumn id="20" xr3:uid="{A1F83970-3B0E-4464-8376-1B37DBE20974}" name="modelType" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{F9DE0808-4FD0-4FB6-9363-B580ED760D5C}" name="model_label" dataDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{2D75E915-5C37-41D0-8D80-E36A15696E43}" name="model_underscore" dataDxfId="117">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE(SUBSTITUTE( co_models[[#This Row],[model_label]], "-", "_" ), " ", "" )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7945,49 +7948,49 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B49:F74" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B49:F74" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
   <autoFilter ref="B49:F74" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B50:F74">
     <sortCondition ref="C50:C74"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="115" totalsRowDxfId="114">
+    <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="114" totalsRowDxfId="113">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CE04D22F-F326-49F0-9B89-F7BBAC07F272}" name="sector_id" dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="4" xr3:uid="{D085A6D5-2B6A-46B4-9638-D837648BB08B}" name="N/A" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="5" xr3:uid="{EB302892-BCFD-4CA5-B470-8D81C8E73DDE}" name="2010" dataDxfId="109" totalsRowDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{FADA0A2C-2C06-4E27-9064-B329CB26787D}" name="2090" dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{CE04D22F-F326-49F0-9B89-F7BBAC07F272}" name="sector_id" dataDxfId="112" totalsRowDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{D085A6D5-2B6A-46B4-9638-D837648BB08B}" name="N/A" dataDxfId="110" totalsRowDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{EB302892-BCFD-4CA5-B470-8D81C8E73DDE}" name="2010" dataDxfId="108" totalsRowDxfId="107"/>
+    <tableColumn id="6" xr3:uid="{FADA0A2C-2C06-4E27-9064-B329CB26787D}" name="2090" dataDxfId="106" totalsRowDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B126:P169" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B126:P169" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
   <autoFilter ref="B126:P169" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B127:P169">
     <sortCondition ref="C127:C169"/>
     <sortCondition ref="D127:D169"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="103">
+    <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="102">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{695E7B0A-9CCF-4B48-8FB4-7B2C8AC23CA2}" name="sector_id" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{AC7D2590-5F6F-4E8A-8395-3ACC925DD65E}" name="impactType_label" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{389F4E81-E357-4437-B986-87606739FD52}" name="impactType_id" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{252ECC08-A081-4155-A2E4-6E6953775245}" name="impactType_description" dataDxfId="99"/>
-    <tableColumn id="18" xr3:uid="{20E67458-91EF-4192-9F05-0BEE3F89945B}" name="physicalmeasure" dataDxfId="98"/>
-    <tableColumn id="6" xr3:uid="{3CFD45D4-B79B-4F80-92FC-337937E46944}" name="physScalarName" dataDxfId="97"/>
-    <tableColumn id="9" xr3:uid="{40E9B945-11EE-47C9-B5D8-A41A8FC63734}" name="physAdjName" dataDxfId="96"/>
-    <tableColumn id="16" xr3:uid="{5C5AE37A-2086-491F-BF3C-F22CC928E516}" name="damageAdjName" dataDxfId="95"/>
-    <tableColumn id="10" xr3:uid="{2A5B466E-A990-49E9-92E3-0103059D4863}" name="econScalarName" dataDxfId="94"/>
-    <tableColumn id="11" xr3:uid="{74F77DB7-A970-4C19-A8F9-04E79FC664FD}" name="econMultiplierName" dataDxfId="93"/>
-    <tableColumn id="12" xr3:uid="{DA200B1A-95FB-4000-933E-BC048A1E0631}" name="c0" dataDxfId="92"/>
-    <tableColumn id="13" xr3:uid="{F6CED4C7-F96B-4766-BD90-7B52A49FAABA}" name="c1" dataDxfId="91"/>
-    <tableColumn id="14" xr3:uid="{E36983CA-3DF1-4DD8-A727-E60C1D905346}" name="exp0" dataDxfId="90"/>
-    <tableColumn id="15" xr3:uid="{861014FE-4437-4D17-8CED-BC8B72417DD9}" name="year0" dataDxfId="89">
+    <tableColumn id="5" xr3:uid="{695E7B0A-9CCF-4B48-8FB4-7B2C8AC23CA2}" name="sector_id" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{AC7D2590-5F6F-4E8A-8395-3ACC925DD65E}" name="impactType_label" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{389F4E81-E357-4437-B986-87606739FD52}" name="impactType_id" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{252ECC08-A081-4155-A2E4-6E6953775245}" name="impactType_description" dataDxfId="98"/>
+    <tableColumn id="18" xr3:uid="{20E67458-91EF-4192-9F05-0BEE3F89945B}" name="physicalmeasure" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{3CFD45D4-B79B-4F80-92FC-337937E46944}" name="physScalarName" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{40E9B945-11EE-47C9-B5D8-A41A8FC63734}" name="physAdjName" dataDxfId="95"/>
+    <tableColumn id="16" xr3:uid="{5C5AE37A-2086-491F-BF3C-F22CC928E516}" name="damageAdjName" dataDxfId="94"/>
+    <tableColumn id="10" xr3:uid="{2A5B466E-A990-49E9-92E3-0103059D4863}" name="econScalarName" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{74F77DB7-A970-4C19-A8F9-04E79FC664FD}" name="econMultiplierName" dataDxfId="92"/>
+    <tableColumn id="12" xr3:uid="{DA200B1A-95FB-4000-933E-BC048A1E0631}" name="c0" dataDxfId="91"/>
+    <tableColumn id="13" xr3:uid="{F6CED4C7-F96B-4766-BD90-7B52A49FAABA}" name="c1" dataDxfId="90"/>
+    <tableColumn id="14" xr3:uid="{E36983CA-3DF1-4DD8-A727-E60C1D905346}" name="exp0" dataDxfId="89"/>
+    <tableColumn id="15" xr3:uid="{861014FE-4437-4D17-8CED-BC8B72417DD9}" name="year0" dataDxfId="88">
       <calculatedColumnFormula xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8642,10 +8645,10 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="M8" sqref="M8"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9154,7 +9157,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>334</v>
+        <v>606</v>
       </c>
       <c r="D13" s="27">
         <v>1</v>
@@ -9350,8 +9353,9 @@
       <c r="E17" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="F17" s="27" t="s">
-        <v>123</v>
+      <c r="F17" s="27" t="str">
+        <f xml:space="preserve"> "row_id"</f>
+        <v>row_id</v>
       </c>
       <c r="G17" s="31" cm="1">
         <f t="array" aca="1" ref="G17" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
@@ -9828,9 +9832,9 @@
   </sheetPr>
   <dimension ref="A1:U333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D274" sqref="D274"/>
+      <selection pane="topRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9964,7 +9968,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C12" s="50" t="str">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_inputScenarioInfo[[#Headers],[row_id]] ), COLUMN( co_inputScenarioInfo[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_inputInfo[[#Headers],[row_id]] ), COLUMN( co_inputInfo[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>Input Scenario Information</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -17406,7 +17410,7 @@
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B264" s="4">
-        <f xml:space="preserve"> ROW( co_inputScenarioInfo[[#This Row],[row_id]] ) - ROW( co_inputScenarioInfo[[#Headers],[row_id]] )</f>
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
       <c r="C264" s="7" t="s">
@@ -17434,7 +17438,7 @@
     </row>
     <row r="265" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B265" s="4">
-        <f xml:space="preserve"> ROW( co_inputScenarioInfo[[#This Row],[row_id]] ) - ROW( co_inputScenarioInfo[[#Headers],[row_id]] )</f>
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
       <c r="C265" s="7" t="s">
@@ -17462,7 +17466,7 @@
     </row>
     <row r="266" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B266" s="4">
-        <f xml:space="preserve"> ROW( co_inputScenarioInfo[[#This Row],[row_id]] ) - ROW( co_inputScenarioInfo[[#Headers],[row_id]] )</f>
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>3</v>
       </c>
       <c r="C266" s="7" t="s">
@@ -17481,7 +17485,7 @@
         <v>0</v>
       </c>
       <c r="H266" s="27" t="str">
-        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
+        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
         <v/>
       </c>
       <c r="I266" s="27" t="s">
@@ -17493,7 +17497,7 @@
     </row>
     <row r="267" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B267" s="4">
-        <f xml:space="preserve"> ROW( co_inputScenarioInfo[[#This Row],[row_id]] ) - ROW( co_inputScenarioInfo[[#Headers],[row_id]] )</f>
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>4</v>
       </c>
       <c r="C267" s="7" t="s">
@@ -17512,7 +17516,7 @@
         <v>0</v>
       </c>
       <c r="H267" s="27" t="str">
-        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputScenarioInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
+        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
         <v/>
       </c>
       <c r="I267" s="27" t="s">
@@ -18584,22 +18588,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B35 B36:F45">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula xml:space="preserve"> IF( $E35 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:F34">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula xml:space="preserve"> IF( $E21 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:F35">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula xml:space="preserve"> IF( $E35 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I132:J132">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula xml:space="preserve"> IF( #REF! = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates to Lyme config
Changes to match formatting standards for Lyme additions in Config file
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B911CEC0-2A3C-4BB8-9BB7-87F9161A8051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62BF34E-9A97-4C70-B778-9E6DBCD7F212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3050,7 +3050,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3296,36 +3296,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="64">
     <cellStyle name="20% - Accent1" xfId="34" builtinId="30" customBuiltin="1"/>
@@ -3394,6 +3364,60 @@
     <cellStyle name="z A Column text" xfId="12" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
   </cellStyles>
   <dxfs count="197">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6240,33 +6264,6 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
@@ -6397,33 +6394,6 @@
         <top/>
         <bottom/>
       </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -7716,38 +7686,38 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B243:D246" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B243:D246" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D7815580-A46D-4035-AF95-6DFB7EDC1C86}" name="row_id" dataDxfId="80">
+    <tableColumn id="1" xr3:uid="{D7815580-A46D-4035-AF95-6DFB7EDC1C86}" name="row_id" dataDxfId="82">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7CEFD3F0-E79C-4BEE-B910-4D600E302386}" name="constant" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{DB7DDBBB-C95A-4211-819C-B05A5C2E7319}" name="value" dataDxfId="78" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{7CEFD3F0-E79C-4BEE-B910-4D600E302386}" name="constant" dataDxfId="81"/>
+    <tableColumn id="3" xr3:uid="{DB7DDBBB-C95A-4211-819C-B05A5C2E7319}" name="value" dataDxfId="80" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B86:I135" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B86:I135" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="B86:I135" xr:uid="{2B645CB4-F641-4C38-A983-F38F00FA7B52}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B87:I135">
     <sortCondition ref="C87:C135"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="75" totalsRowDxfId="74">
+    <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="77" totalsRowDxfId="76">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{11CBE921-72AF-48C1-82DE-27D30284B810}" name="sector_id" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{1A31D87B-CDD5-4D8C-A4C9-8892B2B2C1E8}" name="variant_label" dataDxfId="71" totalsRowDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{BD980D22-60C8-4EA5-878C-1F6646D73814}" name="variant_id" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="7" xr3:uid="{77C8D2EF-4466-45BD-90C6-9DB11F371760}" name="sectorprimary" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{677E6396-DB82-43C2-B1C8-9CF8A385BC06}" name="includeaggregate" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{C16D6C81-A98D-4F3D-B812-6AFD7158219C}" name="damageAdjName" dataDxfId="63" totalsRowDxfId="62">
+    <tableColumn id="18" xr3:uid="{11CBE921-72AF-48C1-82DE-27D30284B810}" name="sector_id" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{1A31D87B-CDD5-4D8C-A4C9-8892B2B2C1E8}" name="variant_label" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{BD980D22-60C8-4EA5-878C-1F6646D73814}" name="variant_id" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{77C8D2EF-4466-45BD-90C6-9DB11F371760}" name="sectorprimary" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{677E6396-DB82-43C2-B1C8-9CF8A385BC06}" name="includeaggregate" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="19" xr3:uid="{C16D6C81-A98D-4F3D-B812-6AFD7158219C}" name="damageAdjName" dataDxfId="65" totalsRowDxfId="64">
       <calculatedColumnFormula xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( co_variants[[#This Row],[sector_id]] = "Roads","_" &amp; co_variants[[#This Row],[variant_id]], "" )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DBDAE92A-E63D-41B7-BD88-AE325DF1F4FE}" name="hasImpacts" dataDxfId="61">
+    <tableColumn id="8" xr3:uid="{DBDAE92A-E63D-41B7-BD88-AE325DF1F4FE}" name="hasImpacts" dataDxfId="63">
       <calculatedColumnFormula array="1" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7756,68 +7726,68 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B235:E238" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B235:E238" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="60">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierDescription" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierDescription" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B285:J289" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B285:J289" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="52">
+    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="54">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{98CB64F8-23F0-4402-9CE1-03695A07036B}" name="inputDesc" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{98CB64F8-23F0-4402-9CE1-03695A07036B}" name="inputDesc" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="48">
       <calculatedColumnFormula xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="region" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="region" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B306:F355" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B306:F355" totalsRowShown="0" headerRowDxfId="45">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="42">
+    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="44">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{F4F2D0D4-82EF-41DF-B43B-E23CB36CF080}" name="region" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{F4F2D0D4-82EF-41DF-B43B-E23CB36CF080}" name="region" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B252:I254" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B252:I254" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{39608CCF-EBE2-4EFA-BA66-990DD890C7D3}" name="row_id" dataDxfId="35">
+    <tableColumn id="1" xr3:uid="{39608CCF-EBE2-4EFA-BA66-990DD890C7D3}" name="row_id" dataDxfId="37">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{24491F20-89B9-4A6B-A87E-CDB3D398E1DA}" name="sector" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{60DDD337-313C-431F-83CE-788A259B2B14}" name="physScalarName" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{AB34CD40-6627-470D-9B2F-2360E9A41A63}" name="econMultiplierName" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{774FF8C9-540D-4647-BB5C-0F27D92917EB}" name="c1" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{6D77C177-ACD8-474A-9CEF-58627396E0D5}" name="exp0" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{45D5B794-1A45-47DA-8A77-45C881CC1B29}" name="c2" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{07C4CFF2-DEE6-4176-813C-12CE016805C3}" name="refYear" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{24491F20-89B9-4A6B-A87E-CDB3D398E1DA}" name="sector" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{60DDD337-313C-431F-83CE-788A259B2B14}" name="physScalarName" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{AB34CD40-6627-470D-9B2F-2360E9A41A63}" name="econMultiplierName" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{774FF8C9-540D-4647-BB5C-0F27D92917EB}" name="c1" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{6D77C177-ACD8-474A-9CEF-58627396E0D5}" name="exp0" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{45D5B794-1A45-47DA-8A77-45C881CC1B29}" name="c2" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{07C4CFF2-DEE6-4176-813C-12CE016805C3}" name="refYear" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7827,10 +7797,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}" name="Readme_adaptations" displayName="Readme_adaptations" ref="B9:E15" totalsRowShown="0">
   <autoFilter ref="B9:E15" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="29">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_adaptations[[#This Row],[row_id]] ) - ROW( Readme_adaptations[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{13712644-0D89-49D5-9571-32BD03BF1BD3}" name="adapt_id"/>
     <tableColumn id="3" xr3:uid="{B89736B7-3040-4F82-B2CC-EB15F47F50B3}" name="adapt_label"/>
   </tableColumns>
@@ -7839,23 +7809,23 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="B3:F5" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="25">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_sectors[[#This Row],[row_id]] ) - ROW( Readme_sectors[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{EF872F1E-6955-405B-B61A-5AA538BA1B9E}" name="testDev" displayName="testDev" ref="B3:E28" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{EF872F1E-6955-405B-B61A-5AA538BA1B9E}" name="testDev" displayName="testDev" ref="B3:E28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="B3:E28" xr:uid="{EF872F1E-6955-405B-B61A-5AA538BA1B9E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:E6">
     <sortCondition descending="1" ref="D4:D6"/>
@@ -7863,12 +7833,12 @@
     <sortCondition ref="C4:C6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4105D57-2925-402A-AD59-A6C04C18DAF5}" name="row_id" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{F4105D57-2925-402A-AD59-A6C04C18DAF5}" name="row_id" dataDxfId="18">
       <calculatedColumnFormula xml:space="preserve"> ROW( testDev[[#This Row],[row_id]] ) - ROW(testDev[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{724C3667-B22B-4E0E-A26D-84EB27DA32DC}" name="Table Name" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{2DE33227-E2C9-4F8F-BDC2-7C7EB619B32B}" name="Changes if new sector added" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{91AE5770-239D-41B2-B469-E73127600B2A}" name="New sector changes" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{724C3667-B22B-4E0E-A26D-84EB27DA32DC}" name="Table Name" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{2DE33227-E2C9-4F8F-BDC2-7C7EB619B32B}" name="Changes if new sector added" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{91AE5770-239D-41B2-B469-E73127600B2A}" name="New sector changes" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7878,17 +7848,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}" name="slr_cm" displayName="slr_cm" ref="A1:I102" totalsRowShown="0">
   <autoFilter ref="A1:I102" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="14">
       <calculatedColumnFormula xml:space="preserve"> ROW( slr_cm[[#This Row],[row_id]] ) - ROW( slr_cm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7965,17 +7935,17 @@
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{031B452A-F7AD-42C2-B528-CC3050A26AA0}" name="interpolateEstimateYears" dataDxfId="155" totalsRowDxfId="154">
-      <calculatedColumnFormula xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{031B452A-F7AD-42C2-B528-CC3050A26AA0}" name="interpolateEstimateYears" dataDxfId="1" totalsRowDxfId="155">
+      <calculatedColumnFormula xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C86349E6-E4A5-4E4F-8866-5A0EC09E18B2}" name="Number of variants" dataDxfId="153" totalsRowDxfId="152">
+    <tableColumn id="10" xr3:uid="{C86349E6-E4A5-4E4F-8866-5A0EC09E18B2}" name="Number of variants" dataDxfId="154" totalsRowDxfId="153">
       <calculatedColumnFormula array="1" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{5F0E2743-320C-46C8-BF83-E0748C4ED15D}" name="Number of impact types" dataDxfId="151" totalsRowDxfId="150">
+    <tableColumn id="11" xr3:uid="{5F0E2743-320C-46C8-BF83-E0748C4ED15D}" name="Number of impact types" dataDxfId="152" totalsRowDxfId="151">
       <calculatedColumnFormula array="1" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{39CDE92C-BE84-47A0-A80A-EB0EC7367742}" name="Number of impact years" dataDxfId="149" totalsRowDxfId="148">
-      <calculatedColumnFormula array="1" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</calculatedColumnFormula>
+    <tableColumn id="13" xr3:uid="{39CDE92C-BE84-47A0-A80A-EB0EC7367742}" name="Number of impact years" dataDxfId="0" totalsRowDxfId="150">
+      <calculatedColumnFormula array="1" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -7983,34 +7953,34 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B259:L261" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B259:L261" totalsRowShown="0" headerRowDxfId="149" dataDxfId="148">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{11DFD282-93A9-4795-9369-6627D14BB282}" name="row_id" dataDxfId="145">
+    <tableColumn id="1" xr3:uid="{11DFD282-93A9-4795-9369-6627D14BB282}" name="row_id" dataDxfId="147">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{083A43A4-471A-4911-84CB-93A1DE17EDC1}" name="modelType_id" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{5A95B322-31B8-49BE-B215-52BB75258F9F}" name="modelType_label" dataDxfId="143"/>
-    <tableColumn id="3" xr3:uid="{540088D4-3239-4E2E-B19D-9DEA7196BB93}" name="inputName" dataDxfId="142"/>
-    <tableColumn id="7" xr3:uid="{EDB25577-4E2B-4262-9DF5-F68DC828D4E8}" name="modelUnitDesc" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{7172DDAD-67EF-469B-A2DF-E5E2773966BC}" name="modelUnit_id" dataDxfId="140"/>
-    <tableColumn id="8" xr3:uid="{0E585296-9334-4F27-8B15-1B944CD33E6C}" name="modelUnit_label" dataDxfId="139"/>
-    <tableColumn id="10" xr3:uid="{5F1496AF-7FEE-4618-AAE6-2E8C8F5433BE}" name="modelUnitScale" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{72573958-4C31-41E8-A620-C05E0EAD6C20}" name="modelRefYear" dataDxfId="137"/>
-    <tableColumn id="14" xr3:uid="{24E03EC5-2F20-4779-B9C9-9AA4430B9341}" name="modelMaxOutput" dataDxfId="136"/>
-    <tableColumn id="9" xr3:uid="{537B6620-4A1F-465E-B24B-88B4E9CB99EF}" name="modelMaxExtrap" dataDxfId="135"/>
+    <tableColumn id="5" xr3:uid="{083A43A4-471A-4911-84CB-93A1DE17EDC1}" name="modelType_id" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{5A95B322-31B8-49BE-B215-52BB75258F9F}" name="modelType_label" dataDxfId="145"/>
+    <tableColumn id="3" xr3:uid="{540088D4-3239-4E2E-B19D-9DEA7196BB93}" name="inputName" dataDxfId="144"/>
+    <tableColumn id="7" xr3:uid="{EDB25577-4E2B-4262-9DF5-F68DC828D4E8}" name="modelUnitDesc" dataDxfId="143"/>
+    <tableColumn id="2" xr3:uid="{7172DDAD-67EF-469B-A2DF-E5E2773966BC}" name="modelUnit_id" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{0E585296-9334-4F27-8B15-1B944CD33E6C}" name="modelUnit_label" dataDxfId="141"/>
+    <tableColumn id="10" xr3:uid="{5F1496AF-7FEE-4618-AAE6-2E8C8F5433BE}" name="modelUnitScale" dataDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{72573958-4C31-41E8-A620-C05E0EAD6C20}" name="modelRefYear" dataDxfId="139"/>
+    <tableColumn id="14" xr3:uid="{24E03EC5-2F20-4779-B9C9-9AA4430B9341}" name="modelMaxOutput" dataDxfId="138"/>
+    <tableColumn id="9" xr3:uid="{537B6620-4A1F-465E-B24B-88B4E9CB99EF}" name="modelMaxExtrap" dataDxfId="137"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B294:D301" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B294:D301" totalsRowShown="0" headerRowDxfId="136" dataDxfId="135">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{18599272-3810-42BA-A220-485AFB1D6807}" name="row_id" dataDxfId="132">
+    <tableColumn id="1" xr3:uid="{18599272-3810-42BA-A220-485AFB1D6807}" name="row_id" dataDxfId="134">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{56B07D04-3458-4687-B04E-181849066DB3}" name="region_label" dataDxfId="131"/>
-    <tableColumn id="5" xr3:uid="{FFA64F27-24E0-4D92-8E8A-6A4675CEB856}" name="region_id" dataDxfId="130">
+    <tableColumn id="3" xr3:uid="{56B07D04-3458-4687-B04E-181849066DB3}" name="region_label" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{FFA64F27-24E0-4D92-8E8A-6A4675CEB856}" name="region_id" dataDxfId="132">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8019,66 +7989,66 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B266:F280" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B266:F280" totalsRowShown="0" headerRowDxfId="131" dataDxfId="130">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="127">
+    <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="129">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A209304D-718C-45BB-922A-A83B3EC89858}" name="model_id" dataDxfId="126">
+    <tableColumn id="2" xr3:uid="{A209304D-718C-45BB-922A-A83B3EC89858}" name="model_id" dataDxfId="128">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CBC70E09-D146-4CF4-911F-60EB221755C0}" name="maxUnitValue" dataDxfId="125"/>
-    <tableColumn id="20" xr3:uid="{A1F83970-3B0E-4464-8376-1B37DBE20974}" name="modelType" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{F9DE0808-4FD0-4FB6-9363-B580ED760D5C}" name="model_label" dataDxfId="123"/>
+    <tableColumn id="5" xr3:uid="{CBC70E09-D146-4CF4-911F-60EB221755C0}" name="maxUnitValue" dataDxfId="127"/>
+    <tableColumn id="20" xr3:uid="{A1F83970-3B0E-4464-8376-1B37DBE20974}" name="modelType" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{F9DE0808-4FD0-4FB6-9363-B580ED760D5C}" name="model_label" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B52:F80" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B52:F80" totalsRowShown="0" headerRowDxfId="124" dataDxfId="123">
   <autoFilter ref="B52:F80" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B53:F80">
     <sortCondition ref="C53:C80"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="120" totalsRowDxfId="119">
+    <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="122" totalsRowDxfId="121">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CE04D22F-F326-49F0-9B89-F7BBAC07F272}" name="sector_id" dataDxfId="118" totalsRowDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{D085A6D5-2B6A-46B4-9638-D837648BB08B}" name="NA" dataDxfId="116" totalsRowDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{EB302892-BCFD-4CA5-B470-8D81C8E73DDE}" name="2010" dataDxfId="114" totalsRowDxfId="113"/>
-    <tableColumn id="6" xr3:uid="{FADA0A2C-2C06-4E27-9064-B329CB26787D}" name="2090" dataDxfId="112" totalsRowDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{CE04D22F-F326-49F0-9B89-F7BBAC07F272}" name="sector_id" dataDxfId="120" totalsRowDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{D085A6D5-2B6A-46B4-9638-D837648BB08B}" name="NA" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{EB302892-BCFD-4CA5-B470-8D81C8E73DDE}" name="2010" dataDxfId="116" totalsRowDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{FADA0A2C-2C06-4E27-9064-B329CB26787D}" name="2090" dataDxfId="114" totalsRowDxfId="113"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B139:P188" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B139:P188" totalsRowShown="0" headerRowDxfId="112" dataDxfId="111">
   <autoFilter ref="B139:P188" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B140:P188">
     <sortCondition ref="C140:C188"/>
     <sortCondition ref="D140:D188"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="110">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{695E7B0A-9CCF-4B48-8FB4-7B2C8AC23CA2}" name="sector_id" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{AC7D2590-5F6F-4E8A-8395-3ACC925DD65E}" name="impactType_label" dataDxfId="106"/>
-    <tableColumn id="2" xr3:uid="{389F4E81-E357-4437-B986-87606739FD52}" name="impactType_id" dataDxfId="105"/>
-    <tableColumn id="7" xr3:uid="{252ECC08-A081-4155-A2E4-6E6953775245}" name="impactType_description" dataDxfId="104"/>
-    <tableColumn id="18" xr3:uid="{20E67458-91EF-4192-9F05-0BEE3F89945B}" name="physicalmeasure" dataDxfId="103"/>
-    <tableColumn id="6" xr3:uid="{3CFD45D4-B79B-4F80-92FC-337937E46944}" name="physScalarName" dataDxfId="102"/>
-    <tableColumn id="9" xr3:uid="{40E9B945-11EE-47C9-B5D8-A41A8FC63734}" name="physAdjName" dataDxfId="101"/>
-    <tableColumn id="16" xr3:uid="{5C5AE37A-2086-491F-BF3C-F22CC928E516}" name="damageAdjName" dataDxfId="100"/>
-    <tableColumn id="10" xr3:uid="{2A5B466E-A990-49E9-92E3-0103059D4863}" name="econScalarName" dataDxfId="99"/>
-    <tableColumn id="11" xr3:uid="{74F77DB7-A970-4C19-A8F9-04E79FC664FD}" name="econMultiplierName" dataDxfId="98"/>
-    <tableColumn id="12" xr3:uid="{DA200B1A-95FB-4000-933E-BC048A1E0631}" name="c0" dataDxfId="97"/>
-    <tableColumn id="13" xr3:uid="{F6CED4C7-F96B-4766-BD90-7B52A49FAABA}" name="c1" dataDxfId="96"/>
-    <tableColumn id="14" xr3:uid="{E36983CA-3DF1-4DD8-A727-E60C1D905346}" name="exp0" dataDxfId="95"/>
-    <tableColumn id="15" xr3:uid="{861014FE-4437-4D17-8CED-BC8B72417DD9}" name="year0" dataDxfId="94">
+    <tableColumn id="5" xr3:uid="{695E7B0A-9CCF-4B48-8FB4-7B2C8AC23CA2}" name="sector_id" dataDxfId="109"/>
+    <tableColumn id="3" xr3:uid="{AC7D2590-5F6F-4E8A-8395-3ACC925DD65E}" name="impactType_label" dataDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{389F4E81-E357-4437-B986-87606739FD52}" name="impactType_id" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{252ECC08-A081-4155-A2E4-6E6953775245}" name="impactType_description" dataDxfId="106"/>
+    <tableColumn id="18" xr3:uid="{20E67458-91EF-4192-9F05-0BEE3F89945B}" name="physicalmeasure" dataDxfId="105"/>
+    <tableColumn id="6" xr3:uid="{3CFD45D4-B79B-4F80-92FC-337937E46944}" name="physScalarName" dataDxfId="104"/>
+    <tableColumn id="9" xr3:uid="{40E9B945-11EE-47C9-B5D8-A41A8FC63734}" name="physAdjName" dataDxfId="103"/>
+    <tableColumn id="16" xr3:uid="{5C5AE37A-2086-491F-BF3C-F22CC928E516}" name="damageAdjName" dataDxfId="102"/>
+    <tableColumn id="10" xr3:uid="{2A5B466E-A990-49E9-92E3-0103059D4863}" name="econScalarName" dataDxfId="101"/>
+    <tableColumn id="11" xr3:uid="{74F77DB7-A970-4C19-A8F9-04E79FC664FD}" name="econMultiplierName" dataDxfId="100"/>
+    <tableColumn id="12" xr3:uid="{DA200B1A-95FB-4000-933E-BC048A1E0631}" name="c0" dataDxfId="99"/>
+    <tableColumn id="13" xr3:uid="{F6CED4C7-F96B-4766-BD90-7B52A49FAABA}" name="c1" dataDxfId="98"/>
+    <tableColumn id="14" xr3:uid="{E36983CA-3DF1-4DD8-A727-E60C1D905346}" name="exp0" dataDxfId="97"/>
+    <tableColumn id="15" xr3:uid="{861014FE-4437-4D17-8CED-BC8B72417DD9}" name="year0" dataDxfId="96">
       <calculatedColumnFormula xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8087,24 +8057,24 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B193:J230" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B193:J230" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="B193:J230" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B194:J225">
     <sortCondition ref="E194:E225"/>
     <sortCondition ref="C194:C225"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="91">
+    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="93">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarName" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{11586BC8-9866-411F-AFB1-B54CDBE58BC8}" name="scalarLabel" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{59273865-10D7-4E58-A34B-98B12FD27367}" name="scalarType" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{44722630-DE32-4127-9D36-E5716D7B6FB1}" name="constant_or_dynamic" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{06B55EB3-A830-4A09-BCEF-732F610DB775}" name="national_or_regional" dataDxfId="86"/>
-    <tableColumn id="12" xr3:uid="{DA5FA732-C673-49CC-B393-EEDF239C5944}" name="valueYear" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{072DFA28-3A99-48D9-9F87-0B9663CC8EBE}" name="dataType" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{083C27B7-8723-4638-8D25-C880E916AEB0}" name="notes" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarName" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{11586BC8-9866-411F-AFB1-B54CDBE58BC8}" name="scalarLabel" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{59273865-10D7-4E58-A34B-98B12FD27367}" name="scalarType" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{44722630-DE32-4127-9D36-E5716D7B6FB1}" name="constant_or_dynamic" dataDxfId="89"/>
+    <tableColumn id="7" xr3:uid="{06B55EB3-A830-4A09-BCEF-732F610DB775}" name="national_or_regional" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{DA5FA732-C673-49CC-B393-EEDF239C5944}" name="valueYear" dataDxfId="87"/>
+    <tableColumn id="9" xr3:uid="{072DFA28-3A99-48D9-9F87-0B9663CC8EBE}" name="dataType" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{083C27B7-8723-4638-8D25-C880E916AEB0}" name="notes" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9513,9 +9483,9 @@
   </sheetPr>
   <dimension ref="A1:U355"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H34" sqref="H34"/>
+      <selection pane="topRight" activeCell="I207" sqref="I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9787,8 +9757,8 @@
         <v>Ozone, PM2.5</v>
       </c>
       <c r="J21" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K21" s="36" cm="1">
         <f t="array" ref="K21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -9799,8 +9769,8 @@
         <v>2</v>
       </c>
       <c r="M21" s="36" cm="1">
-        <f t="array" ref="M21" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M21" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
@@ -9839,8 +9809,8 @@
         <v>N/A</v>
       </c>
       <c r="J22" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K22" s="36" cm="1">
         <f t="array" ref="K22" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -9851,8 +9821,8 @@
         <v>1</v>
       </c>
       <c r="M22" s="36" cm="1">
-        <f t="array" ref="M22" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M22" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
@@ -9891,8 +9861,8 @@
         <v>N/A</v>
       </c>
       <c r="J23" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K23" s="36" cm="1">
         <f t="array" ref="K23" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -9903,8 +9873,8 @@
         <v>1</v>
       </c>
       <c r="M23" s="36" cm="1">
-        <f t="array" ref="M23" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M23" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
@@ -9943,8 +9913,8 @@
         <v>Cotton, Maize, Soybean, Wheat</v>
       </c>
       <c r="J24" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K24" s="36" cm="1">
         <f t="array" ref="K24" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -9955,8 +9925,8 @@
         <v>4</v>
       </c>
       <c r="M24" s="36" cm="1">
-        <f t="array" ref="M24" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M24" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
@@ -9995,8 +9965,8 @@
         <v>Property, Violent</v>
       </c>
       <c r="J25" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K25" s="36" cm="1">
         <f t="array" ref="K25" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10007,8 +9977,8 @@
         <v>2</v>
       </c>
       <c r="M25" s="36" cm="1">
-        <f t="array" ref="M25" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M25" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
@@ -10047,8 +10017,8 @@
         <v>N/A</v>
       </c>
       <c r="J26" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K26" s="36" cm="1">
         <f t="array" ref="K26" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10059,8 +10029,8 @@
         <v>1</v>
       </c>
       <c r="M26" s="36" cm="1">
-        <f t="array" ref="M26" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M26" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
@@ -10099,8 +10069,8 @@
         <v>N/A</v>
       </c>
       <c r="J27" s="22">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K27" s="36" cm="1">
         <f t="array" ref="K27" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10111,8 +10081,8 @@
         <v>1</v>
       </c>
       <c r="M27" s="36" cm="1">
-        <f t="array" ref="M27" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M27" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
@@ -10151,8 +10121,8 @@
         <v>N/A</v>
       </c>
       <c r="J28" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K28" s="36" cm="1">
         <f t="array" ref="K28" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10163,8 +10133,8 @@
         <v>1</v>
       </c>
       <c r="M28" s="36" cm="1">
-        <f t="array" ref="M28" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M28" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
@@ -10203,8 +10173,8 @@
         <v>N/A</v>
       </c>
       <c r="J29" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K29" s="36" cm="1">
         <f t="array" ref="K29" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10215,8 +10185,8 @@
         <v>1</v>
       </c>
       <c r="M29" s="36" cm="1">
-        <f t="array" ref="M29" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M29" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
@@ -10255,7 +10225,7 @@
         <v>Cold, Hot</v>
       </c>
       <c r="J30" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>1</v>
       </c>
       <c r="K30" s="36" cm="1">
@@ -10267,7 +10237,7 @@
         <v>2</v>
       </c>
       <c r="M30" s="36" cm="1">
-        <f t="array" ref="M30" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
+        <f t="array" ref="M30" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>2</v>
       </c>
     </row>
@@ -10307,8 +10277,8 @@
         <v>N/A</v>
       </c>
       <c r="J31" s="22">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K31" s="36" cm="1">
         <f t="array" ref="K31" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10319,8 +10289,8 @@
         <v>1</v>
       </c>
       <c r="M31" s="36" cm="1">
-        <f t="array" ref="M31" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M31" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
@@ -10359,8 +10329,8 @@
         <v>N/A</v>
       </c>
       <c r="J32" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K32" s="36" cm="1">
         <f t="array" ref="K32" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10371,8 +10341,8 @@
         <v>1</v>
       </c>
       <c r="M32" s="36" cm="1">
-        <f t="array" ref="M32" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M32" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.2">
@@ -10411,8 +10381,8 @@
         <v>N/A</v>
       </c>
       <c r="J33" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K33" s="36" cm="1">
         <f t="array" ref="K33" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10423,8 +10393,8 @@
         <v>1</v>
       </c>
       <c r="M33" s="36" cm="1">
-        <f t="array" ref="M33" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M33" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.2">
@@ -10463,8 +10433,8 @@
         <v>N/A</v>
       </c>
       <c r="J34" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K34" s="89" cm="1">
         <f t="array" ref="K34" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10475,8 +10445,8 @@
         <v>1</v>
       </c>
       <c r="M34" s="89" cm="1">
-        <f t="array" ref="M34" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M34" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.2">
@@ -10515,8 +10485,8 @@
         <v>N/A</v>
       </c>
       <c r="J35" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K35" s="36" cm="1">
         <f t="array" ref="K35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10527,8 +10497,8 @@
         <v>1</v>
       </c>
       <c r="M35" s="36" cm="1">
-        <f t="array" ref="M35" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M35" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
@@ -10567,8 +10537,8 @@
         <v>Lost Carbon Sequestration, Lost Methane Sequestration, Lost Marsh Area, Property Protection Costs</v>
       </c>
       <c r="J36" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K36" s="89" cm="1">
         <f t="array" ref="K36" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10579,8 +10549,8 @@
         <v>4</v>
       </c>
       <c r="M36" s="89" cm="1">
-        <f t="array" ref="M36" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M36" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
@@ -10619,8 +10589,8 @@
         <v>Restoration Costs</v>
       </c>
       <c r="J37" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K37" s="89" cm="1">
         <f t="array" ref="K37" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10631,8 +10601,8 @@
         <v>1</v>
       </c>
       <c r="M37" s="89" cm="1">
-        <f t="array" ref="M37" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M37" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.2">
@@ -10671,8 +10641,8 @@
         <v>N/A</v>
       </c>
       <c r="J38" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K38" s="36" cm="1">
         <f t="array" ref="K38" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10683,8 +10653,8 @@
         <v>1</v>
       </c>
       <c r="M38" s="36" cm="1">
-        <f t="array" ref="M38" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M38" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
@@ -10723,8 +10693,8 @@
         <v>N/A</v>
       </c>
       <c r="J39" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K39" s="36" cm="1">
         <f t="array" ref="K39" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10735,8 +10705,8 @@
         <v>1</v>
       </c>
       <c r="M39" s="36" cm="1">
-        <f t="array" ref="M39" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M39" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
@@ -10775,8 +10745,8 @@
         <v>N/A</v>
       </c>
       <c r="J40" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K40" s="36" cm="1">
         <f t="array" ref="K40" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10787,8 +10757,8 @@
         <v>1</v>
       </c>
       <c r="M40" s="36" cm="1">
-        <f t="array" ref="M40" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M40" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
@@ -10827,7 +10797,7 @@
         <v>Acute Myocardial Infarction, All Cardiovascular, All Mortality, All Respiratory, Asthma ER</v>
       </c>
       <c r="J41" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>1</v>
       </c>
       <c r="K41" s="36" cm="1">
@@ -10839,7 +10809,7 @@
         <v>5</v>
       </c>
       <c r="M41" s="36" cm="1">
-        <f t="array" ref="M41" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
+        <f t="array" ref="M41" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>2</v>
       </c>
     </row>
@@ -10879,8 +10849,8 @@
         <v>N/A</v>
       </c>
       <c r="J42" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K42" s="36" cm="1">
         <f t="array" ref="K42" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10891,8 +10861,8 @@
         <v>1</v>
       </c>
       <c r="M42" s="36" cm="1">
-        <f t="array" ref="M42" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M42" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
@@ -10931,8 +10901,8 @@
         <v>Lost Wages, Morbidity, Mortality</v>
       </c>
       <c r="J43" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K43" s="36" cm="1">
         <f t="array" ref="K43" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10943,8 +10913,8 @@
         <v>3</v>
       </c>
       <c r="M43" s="36" cm="1">
-        <f t="array" ref="M43" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M43" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
@@ -10983,8 +10953,8 @@
         <v>Direct Medical Cost, Lost Days, Mortality</v>
       </c>
       <c r="J44" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K44" s="36" cm="1">
         <f t="array" ref="K44" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -10995,8 +10965,8 @@
         <v>3</v>
       </c>
       <c r="M44" s="36" cm="1">
-        <f t="array" ref="M44" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M44" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.2">
@@ -11035,8 +11005,8 @@
         <v>N/A</v>
       </c>
       <c r="J45" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K45" s="36" cm="1">
         <f t="array" ref="K45" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -11047,8 +11017,8 @@
         <v>1</v>
       </c>
       <c r="M45" s="36" cm="1">
-        <f t="array" ref="M45" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M45" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
@@ -11087,8 +11057,8 @@
         <v>Morbidity, Mortality, Response Costs</v>
       </c>
       <c r="J46" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K46" s="36" cm="1">
         <f t="array" ref="K46" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -11099,8 +11069,8 @@
         <v>3</v>
       </c>
       <c r="M46" s="36" cm="1">
-        <f t="array" ref="M46" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M46" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
@@ -11139,8 +11109,8 @@
         <v>N/A</v>
       </c>
       <c r="J47" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
-        <v>1</v>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
+        <v>0</v>
       </c>
       <c r="K47" s="36" cm="1">
         <f t="array" ref="K47" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
@@ -11151,8 +11121,8 @@
         <v>1</v>
       </c>
       <c r="M47" s="36" cm="1">
-        <f t="array" ref="M47" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
-        <v>2</v>
+        <f t="array" ref="M47" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
@@ -11191,7 +11161,7 @@
         <v>Alpine Skiing, Cross-Country Skiing, Snowmobiling</v>
       </c>
       <c r="J48" s="21">
-        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "N/A", 0, 1)</f>
+        <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>1</v>
       </c>
       <c r="K48" s="36" cm="1">
@@ -11203,7 +11173,7 @@
         <v>3</v>
       </c>
       <c r="M48" s="36" cm="1">
-        <f t="array" ref="M48" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "N/A", 1, 2 )</f>
+        <f t="array" ref="M48" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>2</v>
       </c>
     </row>
@@ -12725,7 +12695,7 @@
       <c r="M112"/>
     </row>
     <row r="113" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B113" s="91">
+      <c r="B113" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>27</v>
       </c>
@@ -12736,20 +12706,20 @@
         <v>38</v>
       </c>
       <c r="E113" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="F113" s="92">
-        <v>1</v>
-      </c>
-      <c r="G113" s="92">
-        <v>1</v>
-      </c>
-      <c r="H113" s="93" t="str">
+        <v>207</v>
+      </c>
+      <c r="F113" s="61">
+        <v>1</v>
+      </c>
+      <c r="G113" s="61">
+        <v>1</v>
+      </c>
+      <c r="H113" s="47" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( co_variants[[#This Row],[sector_id]] = "Roads","_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I113" s="94" cm="1">
+      <c r="I113" s="34" cm="1">
         <f t="array" ref="I113" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -14515,18 +14485,18 @@
       </c>
     </row>
     <row r="159" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B159" s="91">
+      <c r="B159" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>20</v>
       </c>
-      <c r="C159" s="95" t="s">
+      <c r="C159" s="7" t="s">
         <v>632</v>
       </c>
       <c r="D159" s="28" t="s">
         <v>38</v>
       </c>
       <c r="E159" s="48" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="F159" s="32" t="s">
         <v>634</v>
@@ -14546,7 +14516,7 @@
       <c r="K159" s="28" t="s">
         <v>636</v>
       </c>
-      <c r="L159" s="96" t="s">
+      <c r="L159" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M159" s="27">
@@ -14558,7 +14528,7 @@
       <c r="O159" s="27">
         <v>1</v>
       </c>
-      <c r="P159" s="97" t="str">
+      <c r="P159" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
@@ -16447,7 +16417,7 @@
       </c>
     </row>
     <row r="207" spans="2:19" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B207" s="98">
+      <c r="B207" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>14</v>
       </c>
@@ -16466,10 +16436,10 @@
       <c r="G207" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H207" s="99">
+      <c r="H207" s="81">
         <v>2015</v>
       </c>
-      <c r="I207" s="100" t="s">
+      <c r="I207" s="49" t="s">
         <v>191</v>
       </c>
       <c r="J207" s="66"/>
@@ -19038,22 +19008,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B38 B39:F48">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula xml:space="preserve"> IF( $E38 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:F37">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula xml:space="preserve"> IF( $E21 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:F38">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula xml:space="preserve"> IF( $E38 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I145:J145">
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula xml:space="preserve"> IF( #REF! = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Various changes to the finished "new" sectors
Marsh Migration: switched primary sector to Restoration Costs from Ecosystem Services, removed GHG unit cost scalars to only present physical sequestration measure - this involved changes to the config file (reassigning impactTypes to sector names, removing GHG unit cost scalars, assigning a 0 to c1 for sequestration so it is NOT summed) , removing the GHG unit costs from the scalars folder, and replacing old scaled impacts files with new ones in the gcm folder
Lyme: including "reg_pop" as an internal physical scalar - lyme scaled impacts is per capita
Outdoor Recreation: multiplying scaled impacts by -1 to present losses as positive
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CAC697-69D9-4C31-B42C-2CF8D1507338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC9458D-DA84-436E-88EA-485645A35402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="slr_cm" sheetId="49" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="k_coBillions">controlTables!$D$256</definedName>
-    <definedName name="k_coMillions">controlTables!$D$257</definedName>
-    <definedName name="k_coThousands">controlTables!$D$258</definedName>
+    <definedName name="k_coBillions">controlTables!$D$254</definedName>
+    <definedName name="k_coMillions">controlTables!$D$255</definedName>
+    <definedName name="k_coThousands">controlTables!$D$256</definedName>
     <definedName name="list_co_gcms">co_models[model_id]</definedName>
     <definedName name="list_coimpactYearOptions" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_impactYears[[#Headers],[row_id]] ), COLUMN(co_impactYears[[#Headers],[2090]]), , , "DropDownMenus" ) ), 1, 0, mv_coNum_impactYears, 1 )</definedName>
     <definedName name="loc_coAdaptations">co_variants[[#Headers],[row_id]]</definedName>
@@ -196,7 +196,7 @@
     This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</t>
       </text>
     </comment>
-    <comment ref="J271" authorId="8" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+    <comment ref="J269" authorId="8" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -204,7 +204,7 @@
     Year when change and impacts are zero</t>
       </text>
     </comment>
-    <comment ref="L271" authorId="9" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+    <comment ref="L269" authorId="9" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -212,7 +212,7 @@
     Maximum value to extrapolate to, for models that go up to the maximum output value.</t>
       </text>
     </comment>
-    <comment ref="D278" authorId="10" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+    <comment ref="D276" authorId="10" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -220,7 +220,7 @@
     Max extrapolation temperature</t>
       </text>
     </comment>
-    <comment ref="J297" authorId="11" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+    <comment ref="J295" authorId="11" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="661">
   <si>
     <t>CanESM2</t>
   </si>
@@ -2162,18 +2162,6 @@
   </si>
   <si>
     <t>Restoration Costs</t>
-  </si>
-  <si>
-    <t>unitCost_carbon</t>
-  </si>
-  <si>
-    <t>unitCost_methane</t>
-  </si>
-  <si>
-    <t>Unit Cost of Carbon</t>
-  </si>
-  <si>
-    <t>Unit Cost of Methane</t>
   </si>
   <si>
     <t>Acres of Lost Marsh Area</t>
@@ -3131,7 +3119,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3376,57 +3364,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="64">
@@ -7818,7 +7755,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B255:D258" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{62C1689B-D9D6-412A-917F-C64CA7854F7C}" name="co_constants" displayName="co_constants" ref="B253:D256" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D7815580-A46D-4035-AF95-6DFB7EDC1C86}" name="row_id" dataDxfId="80">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -7858,7 +7795,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B247:E250" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B245:E248" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="58">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -7872,7 +7809,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B297:J301" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B295:J299" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="52">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -7893,7 +7830,7 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B318:F367" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B316:F365" totalsRowShown="0" headerRowDxfId="43">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="42">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -7908,7 +7845,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B264:I266" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{6A7C1084-4BD5-408B-BBB5-2FC0F198D7F4}" name="co_slrScalars" displayName="co_slrScalars" ref="B262:I264" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{39608CCF-EBE2-4EFA-BA66-990DD890C7D3}" name="row_id" dataDxfId="35">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -8085,7 +8022,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B271:L273" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B269:L271" totalsRowShown="0" headerRowDxfId="147" dataDxfId="146">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{11DFD282-93A9-4795-9369-6627D14BB282}" name="row_id" dataDxfId="145">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -8106,7 +8043,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B306:D313" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B304:D311" totalsRowShown="0" headerRowDxfId="134" dataDxfId="133">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18599272-3810-42BA-A220-485AFB1D6807}" name="row_id" dataDxfId="132">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -8121,7 +8058,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B278:F292" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B276:F290" totalsRowShown="0" headerRowDxfId="129" dataDxfId="128">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="127">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -8189,11 +8126,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B202:J242" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
-  <autoFilter ref="B202:J242" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B203:J237">
-    <sortCondition ref="E203:E237"/>
-    <sortCondition ref="C203:C237"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B202:J240" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+  <autoFilter ref="B202:J240" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B203:J235">
+    <sortCondition ref="E203:E235"/>
+    <sortCondition ref="C203:C235"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="91">
@@ -8556,16 +8493,16 @@
   <threadedComment ref="F202" dT="2021-04-02T15:36:58.50" personId="{00000000-0000-0000-0000-000000000000}" id="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
     <text>This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</text>
   </threadedComment>
-  <threadedComment ref="J271" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+  <threadedComment ref="J269" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
     <text>Year when change and impacts are zero</text>
   </threadedComment>
-  <threadedComment ref="L271" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+  <threadedComment ref="L269" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
     <text>Maximum value to extrapolate to, for models that go up to the maximum output value.</text>
   </threadedComment>
-  <threadedComment ref="D278" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+  <threadedComment ref="D276" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
     <text>Max extrapolation temperature</text>
   </threadedComment>
-  <threadedComment ref="J297" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+  <threadedComment ref="J295" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
     <text>Whether region is a dimension of the input</text>
   </threadedComment>
 </ThreadedComments>
@@ -9148,11 +9085,11 @@
       </c>
       <c r="H8" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J8" s="31" cm="1">
         <f t="array" aca="1" ref="J8" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9191,7 +9128,7 @@
       </c>
       <c r="G9" s="31" cm="1">
         <f t="array" aca="1" ref="G9" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H9" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9199,7 +9136,7 @@
       </c>
       <c r="I9" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="J9" s="31" cm="1">
         <f t="array" aca="1" ref="J9" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9238,7 +9175,7 @@
       </c>
       <c r="G10" s="31" cm="1">
         <f t="array" aca="1" ref="G10" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H10" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9246,7 +9183,7 @@
       </c>
       <c r="I10" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J10" s="31" cm="1">
         <f t="array" aca="1" ref="J10" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9285,7 +9222,7 @@
       </c>
       <c r="G11" s="31" cm="1">
         <f t="array" aca="1" ref="G11" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H11" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9293,7 +9230,7 @@
       </c>
       <c r="I11" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J11" s="31" cm="1">
         <f t="array" aca="1" ref="J11" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9335,7 +9272,7 @@
       </c>
       <c r="G12" s="31" cm="1">
         <f t="array" aca="1" ref="G12" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H12" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9343,7 +9280,7 @@
       </c>
       <c r="I12" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J12" s="31" cm="1">
         <f t="array" aca="1" ref="J12" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9382,7 +9319,7 @@
       </c>
       <c r="G13" s="31" cm="1">
         <f t="array" aca="1" ref="G13" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H13" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9390,7 +9327,7 @@
       </c>
       <c r="I13" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J13" s="31" cm="1">
         <f t="array" aca="1" ref="J13" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9523,7 +9460,7 @@
       </c>
       <c r="G16" s="31" cm="1">
         <f t="array" aca="1" ref="G16" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H16" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9531,7 +9468,7 @@
       </c>
       <c r="I16" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="J16" s="31" cm="1">
         <f t="array" aca="1" ref="J16" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9570,7 +9507,7 @@
       </c>
       <c r="G17" s="31" cm="1">
         <f t="array" aca="1" ref="G17" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H17" s="31">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -9578,7 +9515,7 @@
       </c>
       <c r="I17" s="31">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J17" s="31" cm="1">
         <f t="array" aca="1" ref="J17" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -9613,11 +9550,11 @@
   <sheetPr codeName="Sheet15">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U367"/>
+  <dimension ref="A1:U365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D39" sqref="D39"/>
+      <selection pane="topRight" activeCell="N167" sqref="N167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10535,10 +10472,10 @@
         <v>14</v>
       </c>
       <c r="C34" s="76" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="E34" s="12">
         <v>1</v>
@@ -10633,16 +10570,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B36" s="74">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>16</v>
       </c>
       <c r="C36" s="76" t="s">
+        <v>622</v>
+      </c>
+      <c r="D36" s="23" t="s">
         <v>626</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>630</v>
       </c>
       <c r="E36" s="12">
         <v>1</v>
@@ -10666,7 +10603,7 @@
         <f t="array" aca="1" ref="I36" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
-        <v>Lost Carbon Sequestration, Lost Methane Sequestration, Lost Marsh Area, Property Protection Costs</v>
+        <v>Restoration Costs</v>
       </c>
       <c r="J36" s="21">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
@@ -10678,23 +10615,23 @@
       </c>
       <c r="L36" s="89" cm="1">
         <f t="array" ref="L36" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M36" s="89" cm="1">
         <f t="array" ref="M36" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
       <c r="B37" s="74">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>17</v>
       </c>
       <c r="C37" s="76" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="E37" s="12">
         <v>1</v>
@@ -10718,7 +10655,7 @@
         <f t="array" aca="1" ref="I37" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
-        <v>Restoration Costs</v>
+        <v>Lost Carbon Sequestration, Lost Methane Sequestration, Lost Marsh Area, Property Protection Costs</v>
       </c>
       <c r="J37" s="21">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
@@ -10730,7 +10667,7 @@
       </c>
       <c r="L37" s="89" cm="1">
         <f t="array" ref="L37" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M37" s="89" cm="1">
         <f t="array" ref="M37" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
@@ -10738,53 +10675,53 @@
       </c>
     </row>
     <row r="38" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="B38" s="91">
+      <c r="B38" s="74">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>18</v>
       </c>
-      <c r="C38" s="92" t="s">
-        <v>638</v>
-      </c>
-      <c r="D38" s="93" t="s">
-        <v>664</v>
-      </c>
-      <c r="E38" s="94">
-        <v>1</v>
-      </c>
-      <c r="F38" s="95" t="s">
+      <c r="C38" s="76" t="s">
+        <v>634</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>660</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1</v>
+      </c>
+      <c r="F38" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G38" s="96" t="str" cm="1">
+      <c r="G38" s="89" t="str" cm="1">
         <f t="array" aca="1" ref="G38" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_variants[[#Headers],[row_id]] ),  COLUMN( co_variants[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_variants[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_variants[variant_label], "" )
 )</f>
         <v>Proactive Adaptation, No Adaptation</v>
       </c>
-      <c r="H38" s="96" t="str">
+      <c r="H38" s="89" t="str">
         <f ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   OFFSET( INDIRECT( ADDRESS( ROW( INDEX( co_impactYears[sector_id], MATCH( co_sectors[[#This Row],[sector_id]], co_impactYears[sector_id], 0 ) ) ),  COLUMN( co_impactYears[[#Headers],[sector_id]] ), , , "controlTables" ) ), 0, 1, 1, 4 )
 )</f>
         <v>NA</v>
       </c>
-      <c r="I38" s="96" t="str" cm="1">
+      <c r="I38" s="89" t="str" cm="1">
         <f t="array" aca="1" ref="I38" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
         <v>Fishing Activity, Snow Sport Activity, Water Sport Activity, Other Activity, Other Activity Trips</v>
       </c>
-      <c r="J38" s="97">
+      <c r="J38" s="21">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="K38" s="96" cm="1">
+      <c r="K38" s="89" cm="1">
         <f t="array" ref="K38" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="L38" s="96" cm="1">
+      <c r="L38" s="89" cm="1">
         <f t="array" ref="L38" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
         <v>5</v>
       </c>
-      <c r="M38" s="96" cm="1">
+      <c r="M38" s="89" cm="1">
         <f t="array" ref="M38" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>1</v>
       </c>
@@ -11643,7 +11580,7 @@
         <v>14</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D67" s="27" t="s">
         <v>207</v>
@@ -11675,7 +11612,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D69" s="27" t="s">
         <v>207</v>
@@ -11689,7 +11626,7 @@
         <v>17</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D70" s="27" t="s">
         <v>207</v>
@@ -11698,18 +11635,18 @@
       <c r="F70" s="27"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="98">
+      <c r="B71" s="4">
         <f xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</f>
         <v>18</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="D71" s="99" t="s">
+        <v>634</v>
+      </c>
+      <c r="D71" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="E71" s="100"/>
-      <c r="F71" s="99"/>
+      <c r="E71" s="81"/>
+      <c r="F71" s="27"/>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" s="4">
@@ -12898,7 +12835,7 @@
         <v>27</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D115" s="26" t="s">
         <v>38</v>
@@ -12966,10 +12903,10 @@
         <v>29</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D117" s="26" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E117" s="48" t="s">
         <v>602</v>
@@ -13000,10 +12937,10 @@
         <v>30</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D118" s="26" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E118" s="48" t="s">
         <v>601</v>
@@ -13034,10 +12971,10 @@
         <v>31</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D119" s="26" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="E119" s="48" t="s">
         <v>600</v>
@@ -13068,10 +13005,10 @@
         <v>32</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D120" s="26" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="E120" s="48" t="s">
         <v>602</v>
@@ -13102,10 +13039,10 @@
         <v>33</v>
       </c>
       <c r="C121" s="7" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D121" s="26" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E121" s="48" t="s">
         <v>601</v>
@@ -13136,10 +13073,10 @@
         <v>34</v>
       </c>
       <c r="C122" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="D122" s="26" t="s">
         <v>625</v>
-      </c>
-      <c r="D122" s="26" t="s">
-        <v>629</v>
       </c>
       <c r="E122" s="48" t="s">
         <v>600</v>
@@ -13165,12 +13102,12 @@
       <c r="M122"/>
     </row>
     <row r="123" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B123" s="98">
+      <c r="B123" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>35</v>
       </c>
       <c r="C123" s="7" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="D123" s="26" t="s">
         <v>120</v>
@@ -13178,18 +13115,18 @@
       <c r="E123" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="F123" s="101">
-        <v>0</v>
-      </c>
-      <c r="G123" s="101">
-        <v>0</v>
-      </c>
-      <c r="H123" s="102" t="str">
+      <c r="F123" s="61">
+        <v>0</v>
+      </c>
+      <c r="G123" s="61">
+        <v>0</v>
+      </c>
+      <c r="H123" s="47" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( co_variants[[#This Row],[sector_id]] = "Roads","_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I123" s="103" cm="1">
+      <c r="I123" s="34" cm="1">
         <f t="array" ref="I123" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -13199,31 +13136,31 @@
       <c r="M123"/>
     </row>
     <row r="124" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B124" s="98">
+      <c r="B124" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>36</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="D124" s="26" t="s">
         <v>119</v>
       </c>
       <c r="E124" s="48" t="s">
-        <v>639</v>
-      </c>
-      <c r="F124" s="101">
-        <v>1</v>
-      </c>
-      <c r="G124" s="101">
-        <v>1</v>
-      </c>
-      <c r="H124" s="102" t="str">
+        <v>635</v>
+      </c>
+      <c r="F124" s="61">
+        <v>1</v>
+      </c>
+      <c r="G124" s="61">
+        <v>1</v>
+      </c>
+      <c r="H124" s="47" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( co_variants[[#This Row],[sector_id]] = "Roads","_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I124" s="103" cm="1">
+      <c r="I124" s="34" cm="1">
         <f t="array" ref="I124" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -14756,7 +14693,7 @@
         <v>20</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D163" s="28" t="s">
         <v>38</v>
@@ -14765,13 +14702,13 @@
         <v>207</v>
       </c>
       <c r="F163" s="32" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="G163" s="28" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="H163" s="28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I163" s="28" t="s">
         <v>91</v>
@@ -14780,7 +14717,7 @@
         <v>91</v>
       </c>
       <c r="K163" s="28" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="L163" s="28" t="s">
         <v>91</v>
@@ -14854,7 +14791,7 @@
         <v>22</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D165" s="28" t="s">
         <v>613</v>
@@ -14866,7 +14803,7 @@
         <v>611</v>
       </c>
       <c r="G165" s="28" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="H165" s="28" t="s">
         <v>91</v>
@@ -14878,7 +14815,7 @@
         <v>91</v>
       </c>
       <c r="K165" s="28" t="s">
-        <v>618</v>
+        <v>91</v>
       </c>
       <c r="L165" s="28" t="s">
         <v>91</v>
@@ -14887,7 +14824,7 @@
         <v>0</v>
       </c>
       <c r="N165" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O165" s="27">
         <v>1</v>
@@ -14903,7 +14840,7 @@
         <v>23</v>
       </c>
       <c r="C166" s="7" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D166" s="28" t="s">
         <v>614</v>
@@ -14915,7 +14852,7 @@
         <v>612</v>
       </c>
       <c r="G166" s="28" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="H166" s="28" t="s">
         <v>91</v>
@@ -14927,7 +14864,7 @@
         <v>91</v>
       </c>
       <c r="K166" s="28" t="s">
-        <v>619</v>
+        <v>91</v>
       </c>
       <c r="L166" s="28" t="s">
         <v>91</v>
@@ -14936,7 +14873,7 @@
         <v>0</v>
       </c>
       <c r="N166" s="27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O166" s="27">
         <v>1</v>
@@ -14952,7 +14889,7 @@
         <v>24</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D167" s="28" t="s">
         <v>615</v>
@@ -14964,7 +14901,7 @@
         <v>608</v>
       </c>
       <c r="G167" s="28" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="H167" s="28" t="s">
         <v>91</v>
@@ -15001,7 +14938,7 @@
         <v>25</v>
       </c>
       <c r="C168" s="7" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D168" s="28" t="s">
         <v>616</v>
@@ -15050,7 +14987,7 @@
         <v>26</v>
       </c>
       <c r="C169" s="7" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D169" s="28" t="s">
         <v>617</v>
@@ -15094,21 +15031,21 @@
       </c>
     </row>
     <row r="170" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B170" s="98">
+      <c r="B170" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>27</v>
       </c>
-      <c r="C170" s="104" t="s">
-        <v>638</v>
+      <c r="C170" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="D170" s="28" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="E170" s="48" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="F170" s="32" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="G170" s="28" t="s">
         <v>38</v>
@@ -15117,13 +15054,13 @@
         <v>87</v>
       </c>
       <c r="I170" s="28" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="J170" s="28" t="s">
         <v>91</v>
       </c>
       <c r="K170" s="28" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="L170" s="28" t="s">
         <v>91</v>
@@ -15137,27 +15074,27 @@
       <c r="O170" s="27">
         <v>1</v>
       </c>
-      <c r="P170" s="105" t="str">
+      <c r="P170" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="171" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B171" s="98">
+      <c r="B171" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>28</v>
       </c>
-      <c r="C171" s="104" t="s">
+      <c r="C171" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="D171" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="D171" s="28" t="s">
-        <v>642</v>
-      </c>
       <c r="E171" s="48" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="F171" s="32" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="G171" s="28" t="s">
         <v>38</v>
@@ -15166,13 +15103,13 @@
         <v>87</v>
       </c>
       <c r="I171" s="28" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="J171" s="28" t="s">
         <v>91</v>
       </c>
       <c r="K171" s="28" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="L171" s="28" t="s">
         <v>91</v>
@@ -15186,27 +15123,27 @@
       <c r="O171" s="27">
         <v>1</v>
       </c>
-      <c r="P171" s="105" t="str">
+      <c r="P171" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="172" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B172" s="98">
+      <c r="B172" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>29</v>
       </c>
-      <c r="C172" s="104" t="s">
-        <v>638</v>
+      <c r="C172" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="E172" s="48" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="F172" s="32" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="G172" s="28" t="s">
         <v>38</v>
@@ -15215,13 +15152,13 @@
         <v>87</v>
       </c>
       <c r="I172" s="28" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="J172" s="28" t="s">
         <v>91</v>
       </c>
       <c r="K172" s="28" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="L172" s="28" t="s">
         <v>91</v>
@@ -15235,27 +15172,27 @@
       <c r="O172" s="27">
         <v>1</v>
       </c>
-      <c r="P172" s="105" t="str">
+      <c r="P172" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="173" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B173" s="98">
+      <c r="B173" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>30</v>
       </c>
-      <c r="C173" s="104" t="s">
-        <v>638</v>
+      <c r="C173" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="D173" s="28" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="E173" s="28" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="F173" s="32" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="G173" s="28" t="s">
         <v>38</v>
@@ -15264,7 +15201,7 @@
         <v>87</v>
       </c>
       <c r="I173" s="28" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="J173" s="28" t="s">
         <v>91</v>
@@ -15284,36 +15221,36 @@
       <c r="O173" s="27">
         <v>1</v>
       </c>
-      <c r="P173" s="105" t="str">
+      <c r="P173" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="174" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B174" s="98">
+      <c r="B174" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>31</v>
       </c>
-      <c r="C174" s="104" t="s">
-        <v>638</v>
+      <c r="C174" s="7" t="s">
+        <v>634</v>
       </c>
       <c r="D174" s="28" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="E174" s="48" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="F174" s="32" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="G174" s="28" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="H174" s="28" t="s">
         <v>87</v>
       </c>
       <c r="I174" s="28" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="J174" s="28" t="s">
         <v>91</v>
@@ -15333,7 +15270,7 @@
       <c r="O174" s="27">
         <v>1</v>
       </c>
-      <c r="P174" s="105" t="str">
+      <c r="P174" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
@@ -16780,15 +16717,15 @@
       <c r="S210"/>
     </row>
     <row r="211" spans="2:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="B211" s="106">
+      <c r="B211" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>9</v>
       </c>
       <c r="C211" s="32" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="D211" s="26" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="E211" s="81" t="s">
         <v>156</v>
@@ -16799,7 +16736,7 @@
       <c r="G211" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H211" s="107">
+      <c r="H211" s="82">
         <v>2015</v>
       </c>
       <c r="I211" s="49" t="s">
@@ -16934,10 +16871,10 @@
         <v>14</v>
       </c>
       <c r="C216" s="32" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D216" s="26" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="E216" s="81" t="s">
         <v>156</v>
@@ -17013,15 +16950,15 @@
       <c r="J218" s="66"/>
     </row>
     <row r="219" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B219" s="106">
+      <c r="B219" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>17</v>
       </c>
       <c r="C219" s="32" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="D219" s="26" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E219" s="81" t="s">
         <v>156</v>
@@ -17032,7 +16969,7 @@
       <c r="G219" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H219" s="107">
+      <c r="H219" s="82">
         <v>2015</v>
       </c>
       <c r="I219" s="49" t="s">
@@ -17040,28 +16977,28 @@
       </c>
       <c r="J219" s="66"/>
     </row>
-    <row r="220" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:19" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B220" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>18</v>
       </c>
       <c r="C220" s="32" t="s">
-        <v>618</v>
+        <v>260</v>
       </c>
       <c r="D220" s="26" t="s">
-        <v>620</v>
+        <v>262</v>
       </c>
       <c r="E220" s="81" t="s">
         <v>156</v>
       </c>
       <c r="F220" s="81" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G220" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H220" s="82">
-        <v>2015</v>
+      <c r="H220" s="82" t="s">
+        <v>225</v>
       </c>
       <c r="I220" s="49" t="s">
         <v>191</v>
@@ -17074,38 +17011,36 @@
         <v>19</v>
       </c>
       <c r="C221" s="32" t="s">
-        <v>619</v>
+        <v>369</v>
       </c>
       <c r="D221" s="26" t="s">
-        <v>621</v>
+        <v>370</v>
       </c>
       <c r="E221" s="81" t="s">
         <v>156</v>
       </c>
       <c r="F221" s="81" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G221" s="81" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H221" s="82">
         <v>2015</v>
       </c>
-      <c r="I221" s="49" t="s">
-        <v>191</v>
-      </c>
+      <c r="I221" s="49"/>
       <c r="J221" s="66"/>
     </row>
-    <row r="222" spans="2:19" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B222" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>20</v>
       </c>
-      <c r="C222" s="32" t="s">
-        <v>260</v>
+      <c r="C222" s="26" t="s">
+        <v>129</v>
       </c>
       <c r="D222" s="26" t="s">
-        <v>262</v>
+        <v>16</v>
       </c>
       <c r="E222" s="81" t="s">
         <v>156</v>
@@ -17116,8 +17051,8 @@
       <c r="G222" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H222" s="82" t="s">
-        <v>225</v>
+      <c r="H222" s="81">
+        <v>2010</v>
       </c>
       <c r="I222" s="49" t="s">
         <v>191</v>
@@ -17130,10 +17065,10 @@
         <v>21</v>
       </c>
       <c r="C223" s="32" t="s">
-        <v>369</v>
+        <v>655</v>
       </c>
       <c r="D223" s="26" t="s">
-        <v>370</v>
+        <v>658</v>
       </c>
       <c r="E223" s="81" t="s">
         <v>156</v>
@@ -17142,12 +17077,14 @@
         <v>128</v>
       </c>
       <c r="G223" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="H223" s="82">
+        <v>182</v>
+      </c>
+      <c r="H223" s="81">
         <v>2015</v>
       </c>
-      <c r="I223" s="49"/>
+      <c r="I223" s="49" t="s">
+        <v>191</v>
+      </c>
       <c r="J223" s="66"/>
     </row>
     <row r="224" spans="2:19" x14ac:dyDescent="0.2">
@@ -17155,11 +17092,11 @@
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>22</v>
       </c>
-      <c r="C224" s="26" t="s">
-        <v>129</v>
+      <c r="C224" s="32" t="s">
+        <v>114</v>
       </c>
       <c r="D224" s="26" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="E224" s="81" t="s">
         <v>156</v>
@@ -17168,9 +17105,9 @@
         <v>128</v>
       </c>
       <c r="G224" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="H224" s="81">
+        <v>183</v>
+      </c>
+      <c r="H224" s="82">
         <v>2010</v>
       </c>
       <c r="I224" s="49" t="s">
@@ -17179,27 +17116,27 @@
       <c r="J224" s="66"/>
     </row>
     <row r="225" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B225" s="106">
+      <c r="B225" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>23</v>
       </c>
       <c r="C225" s="32" t="s">
-        <v>659</v>
+        <v>93</v>
       </c>
       <c r="D225" s="26" t="s">
-        <v>662</v>
+        <v>136</v>
       </c>
       <c r="E225" s="81" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="F225" s="81" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="G225" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="H225" s="100">
-        <v>2015</v>
+        <v>183</v>
+      </c>
+      <c r="H225" s="82" t="s">
+        <v>225</v>
       </c>
       <c r="I225" s="49" t="s">
         <v>191</v>
@@ -17212,47 +17149,49 @@
         <v>24</v>
       </c>
       <c r="C226" s="32" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D226" s="26" t="s">
-        <v>113</v>
+        <v>196</v>
       </c>
       <c r="E226" s="81" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="F226" s="81" t="s">
         <v>128</v>
       </c>
       <c r="G226" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="H226" s="82">
-        <v>2010</v>
+        <v>182</v>
+      </c>
+      <c r="H226" s="81" t="s">
+        <v>38</v>
       </c>
       <c r="I226" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="J226" s="66"/>
-    </row>
-    <row r="227" spans="2:10" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+      <c r="J226" s="66" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="227" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B227" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>25</v>
       </c>
       <c r="C227" s="32" t="s">
-        <v>93</v>
+        <v>280</v>
       </c>
       <c r="D227" s="26" t="s">
-        <v>136</v>
+        <v>255</v>
       </c>
       <c r="E227" s="81" t="s">
         <v>173</v>
       </c>
       <c r="F227" s="81" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G227" s="81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H227" s="82" t="s">
         <v>225</v>
@@ -17262,16 +17201,16 @@
       </c>
       <c r="J227" s="66"/>
     </row>
-    <row r="228" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B228" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>26</v>
       </c>
       <c r="C228" s="32" t="s">
-        <v>91</v>
+        <v>257</v>
       </c>
       <c r="D228" s="26" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
       <c r="E228" s="81" t="s">
         <v>173</v>
@@ -17282,15 +17221,13 @@
       <c r="G228" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="H228" s="81" t="s">
-        <v>38</v>
+      <c r="H228" s="82" t="s">
+        <v>225</v>
       </c>
       <c r="I228" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="J228" s="66" t="s">
-        <v>197</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="J228" s="66"/>
     </row>
     <row r="229" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B229" s="6">
@@ -17298,10 +17235,10 @@
         <v>27</v>
       </c>
       <c r="C229" s="32" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="D229" s="26" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E229" s="81" t="s">
         <v>173</v>
@@ -17320,25 +17257,25 @@
       </c>
       <c r="J229" s="66"/>
     </row>
-    <row r="230" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B230" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>28</v>
       </c>
       <c r="C230" s="32" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="D230" s="26" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="E230" s="81" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F230" s="81" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="G230" s="81" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H230" s="82" t="s">
         <v>225</v>
@@ -17348,25 +17285,25 @@
       </c>
       <c r="J230" s="66"/>
     </row>
-    <row r="231" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B231" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>29</v>
       </c>
       <c r="C231" s="32" t="s">
-        <v>258</v>
+        <v>103</v>
       </c>
       <c r="D231" s="26" t="s">
-        <v>256</v>
+        <v>102</v>
       </c>
       <c r="E231" s="81" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F231" s="81" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="G231" s="81" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H231" s="82" t="s">
         <v>225</v>
@@ -17382,27 +17319,29 @@
         <v>30</v>
       </c>
       <c r="C232" s="32" t="s">
-        <v>278</v>
+        <v>91</v>
       </c>
       <c r="D232" s="26" t="s">
-        <v>277</v>
+        <v>196</v>
       </c>
       <c r="E232" s="81" t="s">
         <v>158</v>
       </c>
       <c r="F232" s="81" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G232" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="H232" s="82" t="s">
-        <v>225</v>
+        <v>182</v>
+      </c>
+      <c r="H232" s="81" t="s">
+        <v>38</v>
       </c>
       <c r="I232" s="49" t="s">
-        <v>191</v>
-      </c>
-      <c r="J232" s="66"/>
+        <v>193</v>
+      </c>
+      <c r="J232" s="66" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="233" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B233" s="6">
@@ -17410,22 +17349,22 @@
         <v>31</v>
       </c>
       <c r="C233" s="32" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="D233" s="26" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="E233" s="81" t="s">
         <v>158</v>
       </c>
       <c r="F233" s="81" t="s">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G233" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="H233" s="82" t="s">
-        <v>225</v>
+      <c r="H233" s="82">
+        <v>2010</v>
       </c>
       <c r="I233" s="49" t="s">
         <v>191</v>
@@ -17438,29 +17377,27 @@
         <v>32</v>
       </c>
       <c r="C234" s="32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D234" s="26" t="s">
-        <v>196</v>
+        <v>48</v>
       </c>
       <c r="E234" s="81" t="s">
         <v>158</v>
       </c>
       <c r="F234" s="81" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="G234" s="81" t="s">
-        <v>182</v>
-      </c>
-      <c r="H234" s="81" t="s">
-        <v>38</v>
+        <v>183</v>
+      </c>
+      <c r="H234" s="82" t="s">
+        <v>225</v>
       </c>
       <c r="I234" s="49" t="s">
-        <v>193</v>
-      </c>
-      <c r="J234" s="66" t="s">
-        <v>197</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="J234" s="66"/>
     </row>
     <row r="235" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B235" s="6">
@@ -17468,10 +17405,10 @@
         <v>33</v>
       </c>
       <c r="C235" s="32" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D235" s="26" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="E235" s="81" t="s">
         <v>158</v>
@@ -17490,19 +17427,19 @@
       </c>
       <c r="J235" s="66"/>
     </row>
-    <row r="236" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B236" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>34</v>
       </c>
       <c r="C236" s="32" t="s">
-        <v>87</v>
+        <v>652</v>
       </c>
       <c r="D236" s="26" t="s">
-        <v>48</v>
+        <v>659</v>
       </c>
       <c r="E236" s="81" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="F236" s="81" t="s">
         <v>184</v>
@@ -17510,40 +17447,38 @@
       <c r="G236" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="H236" s="82" t="s">
-        <v>225</v>
+      <c r="H236" s="82">
+        <v>2015</v>
       </c>
       <c r="I236" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J236" s="66"/>
     </row>
-    <row r="237" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B237" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>35</v>
       </c>
-      <c r="C237" s="32" t="s">
-        <v>86</v>
+      <c r="C237" s="28" t="s">
+        <v>573</v>
       </c>
       <c r="D237" s="26" t="s">
-        <v>139</v>
+        <v>575</v>
       </c>
       <c r="E237" s="81" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="F237" s="81" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="G237" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="H237" s="82">
-        <v>2010</v>
-      </c>
-      <c r="I237" s="49" t="s">
-        <v>191</v>
-      </c>
+      <c r="H237" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="I237" s="49"/>
       <c r="J237" s="66"/>
     </row>
     <row r="238" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
@@ -17551,11 +17486,11 @@
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>36</v>
       </c>
-      <c r="C238" s="32" t="s">
-        <v>656</v>
+      <c r="C238" s="28" t="s">
+        <v>574</v>
       </c>
       <c r="D238" s="26" t="s">
-        <v>663</v>
+        <v>576</v>
       </c>
       <c r="E238" s="81" t="s">
         <v>173</v>
@@ -17566,27 +17501,25 @@
       <c r="G238" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="H238" s="82">
-        <v>2015</v>
-      </c>
-      <c r="I238" s="49" t="s">
-        <v>191</v>
-      </c>
+      <c r="H238" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="I238" s="49"/>
       <c r="J238" s="66"/>
     </row>
-    <row r="239" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B239" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>37</v>
       </c>
-      <c r="C239" s="28" t="s">
-        <v>573</v>
+      <c r="C239" s="32" t="s">
+        <v>436</v>
       </c>
       <c r="D239" s="26" t="s">
-        <v>575</v>
+        <v>437</v>
       </c>
       <c r="E239" s="81" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F239" s="81" t="s">
         <v>184</v>
@@ -17605,11 +17538,11 @@
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>38</v>
       </c>
-      <c r="C240" s="28" t="s">
-        <v>574</v>
+      <c r="C240" s="32" t="s">
+        <v>438</v>
       </c>
       <c r="D240" s="26" t="s">
-        <v>576</v>
+        <v>439</v>
       </c>
       <c r="E240" s="81" t="s">
         <v>173</v>
@@ -17626,565 +17559,551 @@
       <c r="I240" s="49"/>
       <c r="J240" s="66"/>
     </row>
-    <row r="241" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B241" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>39</v>
-      </c>
-      <c r="C241" s="32" t="s">
-        <v>436</v>
-      </c>
-      <c r="D241" s="26" t="s">
-        <v>437</v>
-      </c>
-      <c r="E241" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="F241" s="81" t="s">
-        <v>184</v>
-      </c>
-      <c r="G241" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="H241" s="82" t="s">
-        <v>225</v>
-      </c>
-      <c r="I241" s="49"/>
-      <c r="J241" s="66"/>
-    </row>
-    <row r="242" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B242" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>40</v>
-      </c>
-      <c r="C242" s="32" t="s">
-        <v>438</v>
-      </c>
-      <c r="D242" s="26" t="s">
-        <v>439</v>
-      </c>
-      <c r="E242" s="81" t="s">
-        <v>173</v>
-      </c>
-      <c r="F242" s="81" t="s">
-        <v>184</v>
-      </c>
-      <c r="G242" s="81" t="s">
-        <v>183</v>
-      </c>
-      <c r="H242" s="82" t="s">
-        <v>225</v>
-      </c>
-      <c r="I242" s="49"/>
-      <c r="J242" s="66"/>
-    </row>
-    <row r="245" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A245" s="16"/>
-      <c r="B245" s="17" t="s">
+    <row r="243" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A243" s="16"/>
+      <c r="B243" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="C245" s="17"/>
-      <c r="D245" s="17"/>
-      <c r="E245" s="17"/>
-      <c r="F245" s="17"/>
-      <c r="G245" s="17"/>
-      <c r="H245" s="17"/>
-      <c r="I245" s="17"/>
-      <c r="J245" s="17"/>
-      <c r="K245" s="17"/>
-      <c r="L245" s="17"/>
-      <c r="M245" s="17"/>
-      <c r="N245" s="17"/>
-      <c r="O245" s="17"/>
-      <c r="P245" s="17"/>
-      <c r="Q245" s="17"/>
-      <c r="R245" s="17"/>
-      <c r="S245" s="17"/>
-      <c r="T245" s="17"/>
-      <c r="U245" s="17"/>
+      <c r="C243" s="17"/>
+      <c r="D243" s="17"/>
+      <c r="E243" s="17"/>
+      <c r="F243" s="17"/>
+      <c r="G243" s="17"/>
+      <c r="H243" s="17"/>
+      <c r="I243" s="17"/>
+      <c r="J243" s="17"/>
+      <c r="K243" s="17"/>
+      <c r="L243" s="17"/>
+      <c r="M243" s="17"/>
+      <c r="N243" s="17"/>
+      <c r="O243" s="17"/>
+      <c r="P243" s="17"/>
+      <c r="Q243" s="17"/>
+      <c r="R243" s="17"/>
+      <c r="S243" s="17"/>
+      <c r="T243" s="17"/>
+      <c r="U243" s="17"/>
+    </row>
+    <row r="245" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B245" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C245" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D245" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="E245" s="30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="246" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B246" s="4">
+        <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C246" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D246" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="E246" s="46">
+        <v>2015</v>
+      </c>
     </row>
     <row r="247" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B247" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C247" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="D247" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="E247" s="30" t="s">
-        <v>159</v>
+      <c r="B247" s="4">
+        <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C247" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D247" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="E247" s="46" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="248" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B248" s="4">
         <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="D248" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="E248" s="46">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B249" s="4">
-        <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
+        <v>196</v>
+      </c>
+      <c r="E248" s="46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="251" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A251" s="16"/>
+      <c r="B251" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="C251" s="17"/>
+      <c r="D251" s="17"/>
+      <c r="E251" s="17"/>
+      <c r="F251" s="17"/>
+      <c r="G251" s="17"/>
+      <c r="H251" s="17"/>
+      <c r="I251" s="17"/>
+      <c r="J251" s="17"/>
+      <c r="K251" s="17"/>
+      <c r="L251" s="17"/>
+      <c r="M251" s="17"/>
+      <c r="N251" s="17"/>
+      <c r="O251" s="17"/>
+      <c r="P251" s="17"/>
+      <c r="Q251" s="17"/>
+      <c r="R251" s="17"/>
+      <c r="S251" s="17"/>
+      <c r="T251" s="17"/>
+      <c r="U251" s="17"/>
+    </row>
+    <row r="253" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B253" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C253" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="D253" s="29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="254" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B254" s="4">
+        <f xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C254" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D254" s="85">
+        <f xml:space="preserve"> 10^9</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="255" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B255" s="4">
+        <f xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C249" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D249" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="E249" s="46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B250" s="4">
-        <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C250" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D250" s="45" t="s">
-        <v>196</v>
-      </c>
-      <c r="E250" s="46" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="253" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A253" s="16"/>
-      <c r="B253" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="C253" s="17"/>
-      <c r="D253" s="17"/>
-      <c r="E253" s="17"/>
-      <c r="F253" s="17"/>
-      <c r="G253" s="17"/>
-      <c r="H253" s="17"/>
-      <c r="I253" s="17"/>
-      <c r="J253" s="17"/>
-      <c r="K253" s="17"/>
-      <c r="L253" s="17"/>
-      <c r="M253" s="17"/>
-      <c r="N253" s="17"/>
-      <c r="O253" s="17"/>
-      <c r="P253" s="17"/>
-      <c r="Q253" s="17"/>
-      <c r="R253" s="17"/>
-      <c r="S253" s="17"/>
-      <c r="T253" s="17"/>
-      <c r="U253" s="17"/>
-    </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B255" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C255" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="D255" s="29" t="s">
-        <v>90</v>
+      <c r="C255" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D255" s="85">
+        <f xml:space="preserve"> 10^6</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="256" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B256" s="4">
         <f xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D256" s="85">
-        <f xml:space="preserve"> 10^9</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="257" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B257" s="4">
-        <f xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C257" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D257" s="85">
-        <f xml:space="preserve"> 10^6</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="258" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B258" s="4">
-        <f xml:space="preserve"> ROW( co_constants[[#This Row],[row_id]] ) - ROW( co_constants[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C258" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D258" s="85">
         <v>1000</v>
       </c>
     </row>
-    <row r="261" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A261" s="16"/>
-      <c r="B261" s="17" t="s">
+    <row r="259" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A259" s="16"/>
+      <c r="B259" s="17" t="s">
         <v>546</v>
       </c>
-      <c r="C261" s="17"/>
-      <c r="D261" s="17"/>
-      <c r="E261" s="17"/>
-      <c r="F261" s="17"/>
-      <c r="G261" s="17"/>
-      <c r="H261" s="17"/>
-      <c r="I261" s="17"/>
-      <c r="J261" s="17"/>
-      <c r="K261" s="17"/>
-      <c r="L261" s="17"/>
-      <c r="M261" s="17"/>
-      <c r="N261" s="17"/>
-      <c r="O261" s="17"/>
-      <c r="P261" s="17"/>
-      <c r="Q261" s="17"/>
-      <c r="R261" s="17"/>
-      <c r="S261" s="17"/>
-      <c r="T261" s="17"/>
-      <c r="U261" s="17"/>
+      <c r="C259" s="17"/>
+      <c r="D259" s="17"/>
+      <c r="E259" s="17"/>
+      <c r="F259" s="17"/>
+      <c r="G259" s="17"/>
+      <c r="H259" s="17"/>
+      <c r="I259" s="17"/>
+      <c r="J259" s="17"/>
+      <c r="K259" s="17"/>
+      <c r="L259" s="17"/>
+      <c r="M259" s="17"/>
+      <c r="N259" s="17"/>
+      <c r="O259" s="17"/>
+      <c r="P259" s="17"/>
+      <c r="Q259" s="17"/>
+      <c r="R259" s="17"/>
+      <c r="S259" s="17"/>
+      <c r="T259" s="17"/>
+      <c r="U259" s="17"/>
+    </row>
+    <row r="260" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B260" s="2" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B262" s="2" t="s">
-        <v>547</v>
+      <c r="B262" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C262" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="D262" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E262" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="F262" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G262" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="H262" s="29" t="s">
+        <v>548</v>
+      </c>
+      <c r="I262" s="29" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="263" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B263" s="4">
+        <f xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C263" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D263" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="E263" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="F263" s="45">
+        <v>1</v>
+      </c>
+      <c r="G263" s="45">
+        <v>0.45</v>
+      </c>
+      <c r="H263" s="45">
+        <v>0</v>
+      </c>
+      <c r="I263" s="45">
+        <v>2100</v>
       </c>
     </row>
     <row r="264" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B264" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C264" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="D264" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E264" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="F264" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="G264" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="H264" s="29" t="s">
-        <v>548</v>
-      </c>
-      <c r="I264" s="29" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="265" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B265" s="4">
-        <f xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</f>
-        <v>1</v>
-      </c>
-      <c r="C265" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="D265" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="E265" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="F265" s="45">
-        <v>1</v>
-      </c>
-      <c r="G265" s="45">
-        <v>0.45</v>
-      </c>
-      <c r="H265" s="45">
-        <v>0</v>
-      </c>
-      <c r="I265" s="45">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="266" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B266" s="4">
+      <c r="B264" s="4">
         <f xml:space="preserve"> ROW( co_slrScalars[[#This Row],[row_id]] ) - ROW( co_slrScalars[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C266" s="45" t="s">
+      <c r="C264" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="D266" s="45" t="s">
+      <c r="D264" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E266" s="45" t="s">
+      <c r="E264" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="F266" s="45">
+      <c r="F264" s="45">
         <v>0.16250000000000001</v>
       </c>
-      <c r="G266" s="45">
-        <v>1</v>
-      </c>
-      <c r="H266" s="45">
+      <c r="G264" s="45">
+        <v>1</v>
+      </c>
+      <c r="H264" s="45">
         <v>0.83750000000000002</v>
       </c>
-      <c r="I266" s="45">
+      <c r="I264" s="45">
         <v>2100</v>
       </c>
     </row>
-    <row r="269" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A269" s="16"/>
-      <c r="B269" s="17" t="s">
+    <row r="267" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A267" s="16"/>
+      <c r="B267" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="C269" s="17"/>
-      <c r="D269" s="17"/>
-      <c r="E269" s="17"/>
-      <c r="F269" s="17"/>
-      <c r="G269" s="17"/>
-      <c r="H269" s="17"/>
-      <c r="I269" s="17"/>
-      <c r="J269" s="17"/>
-      <c r="K269" s="17"/>
-      <c r="L269" s="17"/>
-      <c r="M269" s="17"/>
-      <c r="N269" s="17"/>
-      <c r="O269" s="17"/>
-      <c r="P269" s="17"/>
-      <c r="Q269" s="17"/>
-      <c r="R269" s="17"/>
-      <c r="S269" s="17"/>
-      <c r="T269" s="17"/>
-      <c r="U269" s="17"/>
+      <c r="C267" s="17"/>
+      <c r="D267" s="17"/>
+      <c r="E267" s="17"/>
+      <c r="F267" s="17"/>
+      <c r="G267" s="17"/>
+      <c r="H267" s="17"/>
+      <c r="I267" s="17"/>
+      <c r="J267" s="17"/>
+      <c r="K267" s="17"/>
+      <c r="L267" s="17"/>
+      <c r="M267" s="17"/>
+      <c r="N267" s="17"/>
+      <c r="O267" s="17"/>
+      <c r="P267" s="17"/>
+      <c r="Q267" s="17"/>
+      <c r="R267" s="17"/>
+      <c r="S267" s="17"/>
+      <c r="T267" s="17"/>
+      <c r="U267" s="17"/>
+    </row>
+    <row r="269" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B269" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C269" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="D269" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="E269" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="F269" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="G269" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="H269" s="39" t="s">
+        <v>239</v>
+      </c>
+      <c r="I269" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="J269" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="K269" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="L269" s="37" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="270" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B270" s="4">
+        <f xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C270" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D270" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E270" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="F270" s="42" t="s">
+        <v>229</v>
+      </c>
+      <c r="G270" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="H270" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="I270" s="43">
+        <v>1</v>
+      </c>
+      <c r="J270" s="43">
+        <v>1995</v>
+      </c>
+      <c r="K270" s="43">
+        <v>6</v>
+      </c>
+      <c r="L270" s="43">
+        <v>30</v>
+      </c>
     </row>
     <row r="271" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B271" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="C271" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="D271" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="E271" s="40" t="s">
-        <v>307</v>
-      </c>
-      <c r="F271" s="40" t="s">
-        <v>236</v>
-      </c>
-      <c r="G271" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="H271" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="I271" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="J271" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="K271" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="L271" s="37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="272" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B272" s="4">
-        <f xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</f>
-        <v>1</v>
-      </c>
-      <c r="C272" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="D272" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="E272" s="42" t="s">
-        <v>308</v>
-      </c>
-      <c r="F272" s="42" t="s">
-        <v>229</v>
-      </c>
-      <c r="G272" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="H272" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="I272" s="43">
-        <v>1</v>
-      </c>
-      <c r="J272" s="43">
-        <v>1995</v>
-      </c>
-      <c r="K272" s="43">
-        <v>6</v>
-      </c>
-      <c r="L272" s="43">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="273" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B273" s="4">
+      <c r="B271" s="4">
         <f xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C273" s="7" t="s">
+      <c r="C271" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D273" s="7" t="s">
+      <c r="D271" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="E273" s="42" t="s">
+      <c r="E271" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="F273" s="42" t="s">
+      <c r="F271" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="G273" s="41" t="s">
+      <c r="G271" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="H273" s="41" t="s">
+      <c r="H271" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="I273" s="43">
+      <c r="I271" s="43">
         <v>25</v>
       </c>
-      <c r="J273" s="43">
+      <c r="J271" s="43">
         <v>2000</v>
       </c>
-      <c r="K273" s="43">
+      <c r="K271" s="43">
         <v>250</v>
       </c>
-      <c r="L273" s="43">
+      <c r="L271" s="43">
         <v>1000</v>
       </c>
     </row>
-    <row r="276" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A276" s="16"/>
-      <c r="B276" s="17" t="s">
+    <row r="274" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A274" s="16"/>
+      <c r="B274" s="17" t="s">
         <v>578</v>
       </c>
-      <c r="C276" s="17"/>
-      <c r="D276" s="17"/>
-      <c r="E276" s="17"/>
-      <c r="F276" s="17"/>
-      <c r="G276" s="17"/>
-      <c r="H276" s="17"/>
-      <c r="I276" s="17"/>
-      <c r="J276" s="17"/>
-      <c r="K276" s="17"/>
-      <c r="L276" s="17"/>
-      <c r="M276" s="17"/>
-      <c r="N276" s="17"/>
-      <c r="O276" s="17"/>
-      <c r="P276" s="17"/>
-      <c r="Q276" s="17"/>
-      <c r="R276" s="17"/>
-      <c r="S276" s="17"/>
-      <c r="T276" s="17"/>
-      <c r="U276" s="17"/>
+      <c r="C274" s="17"/>
+      <c r="D274" s="17"/>
+      <c r="E274" s="17"/>
+      <c r="F274" s="17"/>
+      <c r="G274" s="17"/>
+      <c r="H274" s="17"/>
+      <c r="I274" s="17"/>
+      <c r="J274" s="17"/>
+      <c r="K274" s="17"/>
+      <c r="L274" s="17"/>
+      <c r="M274" s="17"/>
+      <c r="N274" s="17"/>
+      <c r="O274" s="17"/>
+      <c r="P274" s="17"/>
+      <c r="Q274" s="17"/>
+      <c r="R274" s="17"/>
+      <c r="S274" s="17"/>
+      <c r="T274" s="17"/>
+      <c r="U274" s="17"/>
+    </row>
+    <row r="276" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B276" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C276" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="D276" s="29" t="s">
+        <v>545</v>
+      </c>
+      <c r="E276" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F276" s="30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="277" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B277" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C277" s="90" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>CanESM2</v>
+      </c>
+      <c r="D277" s="45">
+        <v>6</v>
+      </c>
+      <c r="E277" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="F277" s="87" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="278" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B278" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C278" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="D278" s="29" t="s">
-        <v>545</v>
-      </c>
-      <c r="E278" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="F278" s="30" t="s">
-        <v>227</v>
+      <c r="B278" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C278" s="90" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>CCSM4</v>
+      </c>
+      <c r="D278" s="45">
+        <v>5</v>
+      </c>
+      <c r="E278" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="F278" s="87" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="279" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B279" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C279" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CanESM2</v>
+        <v>GISSE2R</v>
       </c>
       <c r="D279" s="45">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E279" s="45" t="s">
         <v>161</v>
       </c>
       <c r="F279" s="87" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B280" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C280" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CCSM4</v>
+        <v>HadGEM2ES</v>
       </c>
       <c r="D280" s="45">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E280" s="45" t="s">
         <v>161</v>
       </c>
       <c r="F280" s="87" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="281" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B281" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C281" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GISSE2R</v>
+        <v>MIROC5</v>
       </c>
       <c r="D281" s="45">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E281" s="45" t="s">
         <v>161</v>
       </c>
       <c r="F281" s="87" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B282" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C282" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>HadGEM2ES</v>
+        <v>GFDLCM3</v>
       </c>
       <c r="D282" s="45">
         <v>6</v>
@@ -18193,93 +18112,93 @@
         <v>161</v>
       </c>
       <c r="F282" s="87" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B283" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C283" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MIROC5</v>
+        <v>MRICGCM3</v>
       </c>
       <c r="D283" s="45">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E283" s="45" t="s">
         <v>161</v>
       </c>
       <c r="F283" s="87" t="s">
-        <v>4</v>
+        <v>341</v>
       </c>
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B284" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C284" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GFDLCM3</v>
+        <v>GCMEnsemble</v>
       </c>
       <c r="D284" s="45">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E284" s="45" t="s">
         <v>161</v>
       </c>
       <c r="F284" s="87" t="s">
-        <v>5</v>
+        <v>339</v>
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B285" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C285" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MRICGCM3</v>
+        <v>30cm</v>
       </c>
       <c r="D285" s="45">
-        <v>3</v>
+        <v>250</v>
       </c>
       <c r="E285" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F285" s="87" t="s">
-        <v>341</v>
+        <v>579</v>
       </c>
     </row>
     <row r="286" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B286" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C286" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GCMEnsemble</v>
+        <v>50cm</v>
       </c>
       <c r="D286" s="45">
-        <v>5</v>
+        <v>250</v>
       </c>
       <c r="E286" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F286" s="87" t="s">
-        <v>339</v>
+        <v>580</v>
       </c>
     </row>
     <row r="287" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B287" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C287" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>30cm</v>
+        <v>100cm</v>
       </c>
       <c r="D287" s="45">
         <v>250</v>
@@ -18288,17 +18207,17 @@
         <v>160</v>
       </c>
       <c r="F287" s="87" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="288" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B288" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C288" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>50cm</v>
+        <v>150cm</v>
       </c>
       <c r="D288" s="45">
         <v>250</v>
@@ -18307,17 +18226,17 @@
         <v>160</v>
       </c>
       <c r="F288" s="87" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B289" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C289" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>100cm</v>
+        <v>200cm</v>
       </c>
       <c r="D289" s="45">
         <v>250</v>
@@ -18326,17 +18245,17 @@
         <v>160</v>
       </c>
       <c r="F289" s="87" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B290" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C290" s="90" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>150cm</v>
+        <v>250cm</v>
       </c>
       <c r="D290" s="45">
         <v>250</v>
@@ -18345,124 +18264,145 @@
         <v>160</v>
       </c>
       <c r="F290" s="87" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="291" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B291" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>13</v>
-      </c>
-      <c r="C291" s="90" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>200cm</v>
-      </c>
-      <c r="D291" s="45">
-        <v>250</v>
-      </c>
-      <c r="E291" s="45" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="293" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A293" s="16"/>
+      <c r="B293" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="C293" s="17"/>
+      <c r="D293" s="17"/>
+      <c r="E293" s="17"/>
+      <c r="F293" s="17"/>
+      <c r="G293" s="17"/>
+      <c r="H293" s="17"/>
+      <c r="I293" s="17"/>
+      <c r="J293" s="17"/>
+      <c r="K293" s="17"/>
+      <c r="L293" s="17"/>
+      <c r="M293" s="17"/>
+      <c r="N293" s="17"/>
+      <c r="O293" s="17"/>
+      <c r="P293" s="17"/>
+      <c r="Q293" s="17"/>
+      <c r="R293" s="17"/>
+      <c r="S293" s="17"/>
+      <c r="T293" s="17"/>
+      <c r="U293" s="17"/>
+    </row>
+    <row r="295" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B295" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C295" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="D295" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="E295" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="F295" s="31" t="s">
+        <v>313</v>
+      </c>
+      <c r="G295" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="H295" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="I295" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="J295" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="296" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B296" s="4">
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C296" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D296" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="E296" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="F296" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="G296" s="27">
+        <v>0</v>
+      </c>
+      <c r="H296" s="27"/>
+      <c r="I296" s="27" t="s">
+        <v>325</v>
+      </c>
+      <c r="J296" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B297" s="4">
+        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C297" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="F291" s="87" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="292" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B292" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>14</v>
-      </c>
-      <c r="C292" s="90" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>250cm</v>
-      </c>
-      <c r="D292" s="45">
-        <v>250</v>
-      </c>
-      <c r="E292" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="F292" s="87" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="295" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A295" s="16"/>
-      <c r="B295" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="C295" s="17"/>
-      <c r="D295" s="17"/>
-      <c r="E295" s="17"/>
-      <c r="F295" s="17"/>
-      <c r="G295" s="17"/>
-      <c r="H295" s="17"/>
-      <c r="I295" s="17"/>
-      <c r="J295" s="17"/>
-      <c r="K295" s="17"/>
-      <c r="L295" s="17"/>
-      <c r="M295" s="17"/>
-      <c r="N295" s="17"/>
-      <c r="O295" s="17"/>
-      <c r="P295" s="17"/>
-      <c r="Q295" s="17"/>
-      <c r="R295" s="17"/>
-      <c r="S295" s="17"/>
-      <c r="T295" s="17"/>
-      <c r="U295" s="17"/>
-    </row>
-    <row r="297" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B297" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C297" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="D297" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="E297" s="29" t="s">
-        <v>316</v>
-      </c>
-      <c r="F297" s="31" t="s">
-        <v>313</v>
-      </c>
-      <c r="G297" s="31" t="s">
-        <v>321</v>
-      </c>
-      <c r="H297" s="31" t="s">
-        <v>322</v>
-      </c>
-      <c r="I297" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="J297" s="31" t="s">
-        <v>55</v>
+      <c r="D297" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="E297" s="45" t="s">
+        <v>318</v>
+      </c>
+      <c r="F297" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="G297" s="27">
+        <v>0</v>
+      </c>
+      <c r="H297" s="27"/>
+      <c r="I297" s="27" t="s">
+        <v>326</v>
+      </c>
+      <c r="J297" s="27">
+        <v>0</v>
       </c>
     </row>
     <row r="298" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B298" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C298" s="7" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D298" s="45" t="s">
-        <v>228</v>
+        <v>312</v>
       </c>
       <c r="E298" s="45" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F298" s="27" t="s">
-        <v>234</v>
+        <v>314</v>
       </c>
       <c r="G298" s="27">
         <v>0</v>
       </c>
-      <c r="H298" s="27"/>
+      <c r="H298" s="27" t="str">
+        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
+        <v/>
+      </c>
       <c r="I298" s="27" t="s">
-        <v>325</v>
+        <v>187</v>
       </c>
       <c r="J298" s="27">
         <v>0</v>
@@ -18471,1149 +18411,1090 @@
     <row r="299" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B299" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C299" s="7" t="s">
-        <v>160</v>
+        <v>310</v>
       </c>
       <c r="D299" s="45" t="s">
-        <v>233</v>
+        <v>577</v>
       </c>
       <c r="E299" s="45" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F299" s="27" t="s">
-        <v>235</v>
+        <v>315</v>
       </c>
       <c r="G299" s="27">
         <v>0</v>
       </c>
-      <c r="H299" s="27"/>
-      <c r="I299" s="27" t="s">
-        <v>326</v>
-      </c>
-      <c r="J299" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B300" s="4">
-        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C300" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D300" s="45" t="s">
-        <v>312</v>
-      </c>
-      <c r="E300" s="45" t="s">
-        <v>319</v>
-      </c>
-      <c r="F300" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="G300" s="27">
-        <v>0</v>
-      </c>
-      <c r="H300" s="27" t="str">
+      <c r="H299" s="27" t="str">
         <f xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
         <v/>
       </c>
-      <c r="I300" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="J300" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B301" s="4">
-        <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
-        <v>4</v>
-      </c>
-      <c r="C301" s="7" t="s">
+      <c r="I299" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="D301" s="45" t="s">
-        <v>577</v>
-      </c>
-      <c r="E301" s="45" t="s">
-        <v>320</v>
-      </c>
-      <c r="F301" s="27" t="s">
-        <v>315</v>
-      </c>
-      <c r="G301" s="27">
-        <v>0</v>
-      </c>
-      <c r="H301" s="27" t="str">
-        <f xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[modelMaxExtrap], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</f>
-        <v/>
-      </c>
-      <c r="I301" s="27" t="s">
-        <v>310</v>
-      </c>
-      <c r="J301" s="27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A304" s="16"/>
-      <c r="B304" s="17" t="s">
+      <c r="J299" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A302" s="16"/>
+      <c r="B302" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C304" s="17"/>
-      <c r="D304" s="17"/>
-      <c r="E304" s="17"/>
-      <c r="F304" s="17"/>
-      <c r="G304" s="17"/>
-      <c r="H304" s="17"/>
-      <c r="I304" s="17"/>
-      <c r="J304" s="17"/>
-      <c r="K304" s="17"/>
-      <c r="L304" s="17"/>
-      <c r="M304" s="17"/>
-      <c r="N304" s="17"/>
-      <c r="O304" s="17"/>
-      <c r="P304" s="17"/>
-      <c r="Q304" s="17"/>
-      <c r="R304" s="17"/>
-      <c r="S304" s="17"/>
-      <c r="T304" s="17"/>
-      <c r="U304" s="17"/>
+      <c r="C302" s="17"/>
+      <c r="D302" s="17"/>
+      <c r="E302" s="17"/>
+      <c r="F302" s="17"/>
+      <c r="G302" s="17"/>
+      <c r="H302" s="17"/>
+      <c r="I302" s="17"/>
+      <c r="J302" s="17"/>
+      <c r="K302" s="17"/>
+      <c r="L302" s="17"/>
+      <c r="M302" s="17"/>
+      <c r="N302" s="17"/>
+      <c r="O302" s="17"/>
+      <c r="P302" s="17"/>
+      <c r="Q302" s="17"/>
+      <c r="R302" s="17"/>
+      <c r="S302" s="17"/>
+      <c r="T302" s="17"/>
+      <c r="U302" s="17"/>
+    </row>
+    <row r="304" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B304" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C304" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D304" s="30" t="s">
+        <v>598</v>
+      </c>
+      <c r="E304" s="2"/>
+    </row>
+    <row r="305" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B305" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C305" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D305" s="30" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>Midwest</v>
+      </c>
+      <c r="E305" s="2"/>
     </row>
     <row r="306" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B306" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C306" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D306" s="30" t="s">
-        <v>598</v>
+      <c r="B306" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C306" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D306" s="30" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>Northeast</v>
       </c>
       <c r="E306" s="2"/>
     </row>
     <row r="307" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B307" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C307" s="45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D307" s="30" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Midwest</v>
+        <v>NorthernPlains</v>
       </c>
       <c r="E307" s="2"/>
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B308" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C308" s="45" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D308" s="30" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northeast</v>
+        <v>Northwest</v>
       </c>
       <c r="E308" s="2"/>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B309" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C309" s="45" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D309" s="30" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>NorthernPlains</v>
+        <v>Southeast</v>
       </c>
       <c r="E309" s="2"/>
     </row>
     <row r="310" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B310" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C310" s="45" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D310" s="30" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northwest</v>
+        <v>SouthernPlains</v>
       </c>
       <c r="E310" s="2"/>
     </row>
     <row r="311" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B311" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C311" s="45" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D311" s="30" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Southeast</v>
+        <v>Southwest</v>
       </c>
       <c r="E311" s="2"/>
     </row>
-    <row r="312" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B312" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>6</v>
-      </c>
-      <c r="C312" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D312" s="30" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>SouthernPlains</v>
-      </c>
-      <c r="E312" s="2"/>
-    </row>
-    <row r="313" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B313" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>7</v>
-      </c>
-      <c r="C313" s="45" t="s">
+    <row r="314" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A314" s="16"/>
+      <c r="B314" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="C314" s="17"/>
+      <c r="D314" s="17"/>
+      <c r="E314" s="17"/>
+      <c r="F314" s="17"/>
+      <c r="G314" s="17"/>
+      <c r="H314" s="17"/>
+      <c r="I314" s="17"/>
+      <c r="J314" s="17"/>
+      <c r="K314" s="17"/>
+      <c r="L314" s="17"/>
+      <c r="M314" s="17"/>
+      <c r="N314" s="17"/>
+      <c r="O314" s="17"/>
+      <c r="P314" s="17"/>
+      <c r="Q314" s="17"/>
+      <c r="R314" s="17"/>
+      <c r="S314" s="17"/>
+      <c r="T314" s="17"/>
+      <c r="U314" s="17"/>
+    </row>
+    <row r="316" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B316" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C316" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D316" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E316" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F316" s="9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="317" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B317" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C317" s="83" t="s">
+        <v>445</v>
+      </c>
+      <c r="D317" s="83" t="s">
+        <v>446</v>
+      </c>
+      <c r="E317" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F317" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B318" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C318" s="83" t="s">
+        <v>447</v>
+      </c>
+      <c r="D318" s="83" t="s">
+        <v>448</v>
+      </c>
+      <c r="E318" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="D313" s="30" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Southwest</v>
-      </c>
-      <c r="E313" s="2"/>
-    </row>
-    <row r="316" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A316" s="16"/>
-      <c r="B316" s="17" t="s">
-        <v>441</v>
-      </c>
-      <c r="C316" s="17"/>
-      <c r="D316" s="17"/>
-      <c r="E316" s="17"/>
-      <c r="F316" s="17"/>
-      <c r="G316" s="17"/>
-      <c r="H316" s="17"/>
-      <c r="I316" s="17"/>
-      <c r="J316" s="17"/>
-      <c r="K316" s="17"/>
-      <c r="L316" s="17"/>
-      <c r="M316" s="17"/>
-      <c r="N316" s="17"/>
-      <c r="O316" s="17"/>
-      <c r="P316" s="17"/>
-      <c r="Q316" s="17"/>
-      <c r="R316" s="17"/>
-      <c r="S316" s="17"/>
-      <c r="T316" s="17"/>
-      <c r="U316" s="17"/>
-    </row>
-    <row r="318" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B318" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C318" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D318" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E318" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F318" s="9" t="s">
-        <v>444</v>
+      <c r="F318" s="84">
+        <v>4</v>
       </c>
     </row>
     <row r="319" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B319" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C319" s="83" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="D319" s="83" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="E319" s="83" t="s">
         <v>10</v>
       </c>
       <c r="F319" s="84">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B320" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C320" s="83" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="D320" s="83" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="E320" s="83" t="s">
         <v>12</v>
       </c>
       <c r="F320" s="84">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="321" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B321" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C321" s="83" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="D321" s="83" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="E321" s="83" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F321" s="84">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="322" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B322" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C322" s="83" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D322" s="83" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="E322" s="83" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F322" s="84">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="323" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B323" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C323" s="83" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="D323" s="83" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="E323" s="83" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F323" s="84">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="324" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B324" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C324" s="83" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="D324" s="83" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="E324" s="83" t="s">
         <v>7</v>
       </c>
       <c r="F324" s="84">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="325" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B325" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C325" s="83" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="D325" s="83" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="E325" s="83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F325" s="84">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="326" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B326" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C326" s="83" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="D326" s="83" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E326" s="83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F326" s="84">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="327" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B327" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>11</v>
+      </c>
+      <c r="C327" s="83" t="s">
+        <v>465</v>
+      </c>
+      <c r="D327" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="E327" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="C327" s="83" t="s">
-        <v>461</v>
-      </c>
-      <c r="D327" s="83" t="s">
-        <v>462</v>
-      </c>
-      <c r="E327" s="83" t="s">
-        <v>10</v>
-      </c>
       <c r="F327" s="84">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="328" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B328" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C328" s="83" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D328" s="83" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="E328" s="83" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F328" s="84">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="329" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B329" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C329" s="83" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="D329" s="83" t="s">
-        <v>47</v>
+        <v>469</v>
       </c>
       <c r="E329" s="83" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F329" s="84">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="330" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B330" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C330" s="83" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D330" s="83" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="E330" s="83" t="s">
         <v>6</v>
       </c>
       <c r="F330" s="84">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="331" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B331" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C331" s="83" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="D331" s="83" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="E331" s="83" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F331" s="84">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="332" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B332" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C332" s="83" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="D332" s="83" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="E332" s="83" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F332" s="84">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="333" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B333" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C333" s="83" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="D333" s="83" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="E333" s="83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F333" s="84">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="334" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B334" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C334" s="83" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="D334" s="83" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="E334" s="83" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F334" s="84">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="335" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B335" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C335" s="83" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D335" s="83" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="E335" s="83" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F335" s="84">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="336" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B336" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C336" s="83" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="D336" s="83" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="E336" s="83" t="s">
         <v>7</v>
       </c>
       <c r="F336" s="84">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="337" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B337" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C337" s="83" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="D337" s="83" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="E337" s="83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F337" s="84">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="338" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B338" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C338" s="83" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="D338" s="83" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="E338" s="83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F338" s="84">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="339" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B339" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C339" s="83" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="D339" s="83" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="E339" s="83" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F339" s="84">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="340" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B340" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C340" s="83" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D340" s="83" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="E340" s="83" t="s">
         <v>6</v>
       </c>
       <c r="F340" s="84">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="341" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B341" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C341" s="83" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="D341" s="83" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="E341" s="83" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F341" s="84">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="342" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B342" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C342" s="83" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D342" s="83" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="E342" s="83" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F342" s="84">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="343" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B343" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C343" s="83" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="D343" s="83" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="E343" s="83" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F343" s="84">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="344" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B344" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C344" s="83" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="D344" s="83" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="E344" s="83" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F344" s="84">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="345" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B345" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C345" s="83" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D345" s="83" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="E345" s="83" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F345" s="84">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="346" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B346" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C346" s="83" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="D346" s="83" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="E346" s="83" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F346" s="84">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="347" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B347" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C347" s="83" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D347" s="83" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="E347" s="83" t="s">
         <v>7</v>
       </c>
       <c r="F347" s="84">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="348" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B348" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C348" s="83" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="D348" s="83" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="E348" s="83" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F348" s="84">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="349" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B349" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C349" s="83" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="D349" s="83" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="E349" s="83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F349" s="84">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="350" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B350" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C350" s="83" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="D350" s="83" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="E350" s="83" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F350" s="84">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="351" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B351" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C351" s="83" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="D351" s="83" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="E351" s="83" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F351" s="84">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="352" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B352" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C352" s="83" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="D352" s="83" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="E352" s="83" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F352" s="84">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="353" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B353" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C353" s="83" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="D353" s="83" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="E353" s="83" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F353" s="84">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="354" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B354" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C354" s="83" t="s">
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="D354" s="83" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="E354" s="83" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F354" s="84">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="355" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B355" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C355" s="83" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="D355" s="83" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="E355" s="83" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F355" s="84">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="356" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B356" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C356" s="83" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="D356" s="83" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="E356" s="83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F356" s="84">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="357" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B357" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C357" s="83" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="D357" s="83" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="E357" s="83" t="s">
         <v>10</v>
       </c>
       <c r="F357" s="84">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="358" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B358" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C358" s="83" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="D358" s="83" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="E358" s="83" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F358" s="84">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="359" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B359" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C359" s="83" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="D359" s="83" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="E359" s="83" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F359" s="84">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="360" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B360" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C360" s="83" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="D360" s="83" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="E360" s="83" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F360" s="84">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="361" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B361" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C361" s="83" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="D361" s="83" t="s">
-        <v>529</v>
+        <v>533</v>
       </c>
       <c r="E361" s="83" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F361" s="84">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="362" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B362" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C362" s="83" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="D362" s="83" t="s">
-        <v>531</v>
+        <v>535</v>
       </c>
       <c r="E362" s="83" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F362" s="84">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="363" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B363" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C363" s="83" t="s">
-        <v>532</v>
+        <v>536</v>
       </c>
       <c r="D363" s="83" t="s">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="E363" s="83" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F363" s="84">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="364" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B364" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C364" s="83" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="D364" s="83" t="s">
-        <v>535</v>
+        <v>539</v>
       </c>
       <c r="E364" s="83" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F364" s="84">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="365" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B365" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C365" s="83" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="D365" s="83" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="E365" s="83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F365" s="84">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="366" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B366" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>48</v>
-      </c>
-      <c r="C366" s="83" t="s">
-        <v>538</v>
-      </c>
-      <c r="D366" s="83" t="s">
-        <v>539</v>
-      </c>
-      <c r="E366" s="83" t="s">
-        <v>6</v>
-      </c>
-      <c r="F366" s="84">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="367" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B367" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>49</v>
-      </c>
-      <c r="C367" s="83" t="s">
-        <v>540</v>
-      </c>
-      <c r="D367" s="83" t="s">
-        <v>541</v>
-      </c>
-      <c r="E367" s="83" t="s">
-        <v>8</v>
-      </c>
-      <c r="F367" s="84">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change to gdp/capita value scalar name
changed from gdp_percap to gdp_percap_val
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FEFA8E-9F55-4DA8-91B3-AEBFC26C4719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D555867D-D457-4C3A-928A-2B1834CCDC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1833" uniqueCount="689">
   <si>
     <t>CanESM2</t>
   </si>
@@ -2372,6 +2372,9 @@
   </si>
   <si>
     <t>A.C. purchase and O&amp;M costs to school system</t>
+  </si>
+  <si>
+    <t>gdp_percap_val</t>
   </si>
 </sst>
 </file>
@@ -3206,7 +3209,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3450,63 +3453,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9823,9 +9769,9 @@
   </sheetPr>
   <dimension ref="A1:U384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F29" sqref="F29"/>
+      <selection pane="topRight" activeCell="J168" sqref="J168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10922,62 +10868,62 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="91">
+      <c r="B35" s="73">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>15</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="75" t="s">
         <v>677</v>
       </c>
-      <c r="D35" s="93" t="s">
+      <c r="D35" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="E35" s="94">
-        <v>1</v>
-      </c>
-      <c r="F35" s="95" t="s">
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G35" s="96" t="str" cm="1">
+      <c r="G35" s="88" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_variants[[#Headers],[row_id]] ),  COLUMN( co_variants[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_variants[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_variants[variant_label], "" )
 )</f>
         <v>No Adaptation, Proactive Adaptation</v>
       </c>
-      <c r="H35" s="96" t="str">
+      <c r="H35" s="88" t="str">
         <f ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   OFFSET( INDIRECT( ADDRESS( ROW( INDEX( co_impactYears[sector_id], MATCH( co_sectors[[#This Row],[sector_id]], co_impactYears[sector_id], 0 ) ) ),  COLUMN( co_impactYears[[#Headers],[sector_id]] ), , , "controlTables" ) ), 0, 1, 1, 4 )
 )</f>
         <v>NA</v>
       </c>
-      <c r="I35" s="96" t="str" cm="1">
+      <c r="I35" s="88" t="str" cm="1">
         <f t="array" aca="1" ref="I35" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
         <v>Lost Future Earnings, Adaptation Costs</v>
       </c>
-      <c r="J35" s="97">
+      <c r="J35" s="21">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="K35" s="98" t="b" cm="1">
+      <c r="K35" s="90" t="b" cm="1">
         <f t="array" ref="K35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
         <v>0</v>
       </c>
-      <c r="L35" s="98" t="b" cm="1">
+      <c r="L35" s="90" t="b" cm="1">
         <f t="array" ref="L35" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
       SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c1] &lt;&gt; 0, 1, 0) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
-      <c r="M35" s="96" cm="1">
+      <c r="M35" s="88" cm="1">
         <f t="array" ref="M35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="N35" s="96" cm="1">
+      <c r="N35" s="88" cm="1">
         <f t="array" ref="N35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="O35" s="96" cm="1">
+      <c r="O35" s="88" cm="1">
         <f t="array" ref="O35" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>1</v>
       </c>
@@ -12249,18 +12195,18 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="99">
+      <c r="B70" s="4">
         <f xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</f>
         <v>15</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="D70" s="100" t="s">
+      <c r="D70" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="E70" s="101"/>
-      <c r="F70" s="100"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="27"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="4">
@@ -13586,7 +13532,7 @@
       <c r="M120"/>
     </row>
     <row r="121" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B121" s="99">
+      <c r="B121" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>29</v>
       </c>
@@ -13599,18 +13545,18 @@
       <c r="E121" s="26" t="s">
         <v>635</v>
       </c>
-      <c r="F121" s="102">
-        <v>1</v>
-      </c>
-      <c r="G121" s="102">
-        <v>1</v>
-      </c>
-      <c r="H121" s="103" t="str">
+      <c r="F121" s="60">
+        <v>1</v>
+      </c>
+      <c r="G121" s="60">
+        <v>1</v>
+      </c>
+      <c r="H121" s="46" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I121" s="104" cm="1">
+      <c r="I121" s="34" cm="1">
         <f t="array" ref="I121" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -13620,7 +13566,7 @@
       <c r="M121"/>
     </row>
     <row r="122" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B122" s="99">
+      <c r="B122" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>30</v>
       </c>
@@ -13633,18 +13579,18 @@
       <c r="E122" s="26" t="s">
         <v>679</v>
       </c>
-      <c r="F122" s="102">
-        <v>0</v>
-      </c>
-      <c r="G122" s="102">
-        <v>0</v>
-      </c>
-      <c r="H122" s="103" t="str">
+      <c r="F122" s="60">
+        <v>0</v>
+      </c>
+      <c r="G122" s="60">
+        <v>0</v>
+      </c>
+      <c r="H122" s="46" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I122" s="104" cm="1">
+      <c r="I122" s="34" cm="1">
         <f t="array" ref="I122" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -15394,7 +15340,7 @@
         <v>668</v>
       </c>
       <c r="K168" s="28" t="s">
-        <v>92</v>
+        <v>688</v>
       </c>
       <c r="L168" s="28" t="s">
         <v>91</v>
@@ -15561,11 +15507,11 @@
       </c>
     </row>
     <row r="172" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B172" s="99">
+      <c r="B172" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>21</v>
       </c>
-      <c r="C172" s="105" t="s">
+      <c r="C172" s="7" t="s">
         <v>677</v>
       </c>
       <c r="D172" s="28" t="s">
@@ -15592,7 +15538,7 @@
       <c r="K172" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="L172" s="106" t="s">
+      <c r="L172" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M172" s="27">
@@ -15604,17 +15550,17 @@
       <c r="O172" s="27">
         <v>1</v>
       </c>
-      <c r="P172" s="107" t="str">
+      <c r="P172" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="173" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B173" s="99">
+      <c r="B173" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>22</v>
       </c>
-      <c r="C173" s="105" t="s">
+      <c r="C173" s="7" t="s">
         <v>677</v>
       </c>
       <c r="D173" s="28" t="s">
@@ -15641,7 +15587,7 @@
       <c r="K173" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="L173" s="106" t="s">
+      <c r="L173" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M173" s="27">
@@ -15653,7 +15599,7 @@
       <c r="O173" s="27">
         <v>1</v>
       </c>
-      <c r="P173" s="107" t="str">
+      <c r="P173" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
@@ -17786,7 +17732,7 @@
         <v>12</v>
       </c>
       <c r="C225" s="32" t="s">
-        <v>92</v>
+        <v>688</v>
       </c>
       <c r="D225" s="26" t="s">
         <v>674</v>
@@ -18492,7 +18438,7 @@
       <c r="J249" s="65"/>
     </row>
     <row r="250" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B250" s="108">
+      <c r="B250" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>37</v>
       </c>
@@ -18514,7 +18460,7 @@
       <c r="H250" s="81" t="s">
         <v>225</v>
       </c>
-      <c r="I250" s="109" t="s">
+      <c r="I250" s="48" t="s">
         <v>191</v>
       </c>
       <c r="J250" s="65"/>

</xml_diff>

<commit_message>
Edited test scenario file name
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FEFA8E-9F55-4DA8-91B3-AEBFC26C4719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2009DFE7-AA34-48FF-9CBB-4B33C5E08086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3206,7 +3206,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3452,61 +3452,7 @@
     <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9823,9 +9769,9 @@
   </sheetPr>
   <dimension ref="A1:U384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A269" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F29" sqref="F29"/>
+      <selection pane="topRight" activeCell="K280" sqref="K280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10922,62 +10868,62 @@
       </c>
     </row>
     <row r="35" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="91">
+      <c r="B35" s="73">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>15</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="75" t="s">
         <v>677</v>
       </c>
-      <c r="D35" s="93" t="s">
+      <c r="D35" s="23" t="s">
         <v>678</v>
       </c>
-      <c r="E35" s="94">
-        <v>1</v>
-      </c>
-      <c r="F35" s="95" t="s">
+      <c r="E35" s="12">
+        <v>1</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="G35" s="96" t="str" cm="1">
+      <c r="G35" s="88" t="str" cm="1">
         <f t="array" aca="1" ref="G35" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_variants[[#Headers],[row_id]] ),  COLUMN( co_variants[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_variants[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_variants[variant_label], "" )
 )</f>
         <v>No Adaptation, Proactive Adaptation</v>
       </c>
-      <c r="H35" s="96" t="str">
+      <c r="H35" s="88" t="str">
         <f ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   OFFSET( INDIRECT( ADDRESS( ROW( INDEX( co_impactYears[sector_id], MATCH( co_sectors[[#This Row],[sector_id]], co_impactYears[sector_id], 0 ) ) ),  COLUMN( co_impactYears[[#Headers],[sector_id]] ), , , "controlTables" ) ), 0, 1, 1, 4 )
 )</f>
         <v>NA</v>
       </c>
-      <c r="I35" s="96" t="str" cm="1">
+      <c r="I35" s="88" t="str" cm="1">
         <f t="array" aca="1" ref="I35" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
         <v>Lost Future Earnings, Adaptation Costs</v>
       </c>
-      <c r="J35" s="97">
+      <c r="J35" s="21">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="K35" s="98" t="b" cm="1">
+      <c r="K35" s="90" t="b" cm="1">
         <f t="array" ref="K35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
         <v>0</v>
       </c>
-      <c r="L35" s="98" t="b" cm="1">
+      <c r="L35" s="90" t="b" cm="1">
         <f t="array" ref="L35" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
       SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c1] &lt;&gt; 0, 1, 0) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
-      <c r="M35" s="96" cm="1">
+      <c r="M35" s="91" cm="1">
         <f t="array" ref="M35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="N35" s="96" cm="1">
+      <c r="N35" s="91" cm="1">
         <f t="array" ref="N35" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="O35" s="96" cm="1">
+      <c r="O35" s="91" cm="1">
         <f t="array" ref="O35" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>1</v>
       </c>
@@ -12249,18 +12195,18 @@
       </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="99">
+      <c r="B70" s="4">
         <f xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</f>
         <v>15</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="D70" s="100" t="s">
+      <c r="D70" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="E70" s="101"/>
-      <c r="F70" s="100"/>
+      <c r="E70" s="80"/>
+      <c r="F70" s="27"/>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" s="4">
@@ -13586,7 +13532,7 @@
       <c r="M120"/>
     </row>
     <row r="121" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B121" s="99">
+      <c r="B121" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>29</v>
       </c>
@@ -13599,18 +13545,18 @@
       <c r="E121" s="26" t="s">
         <v>635</v>
       </c>
-      <c r="F121" s="102">
-        <v>1</v>
-      </c>
-      <c r="G121" s="102">
-        <v>1</v>
-      </c>
-      <c r="H121" s="103" t="str">
+      <c r="F121" s="60">
+        <v>1</v>
+      </c>
+      <c r="G121" s="60">
+        <v>1</v>
+      </c>
+      <c r="H121" s="46" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I121" s="104" cm="1">
+      <c r="I121" s="34" cm="1">
         <f t="array" ref="I121" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -13620,7 +13566,7 @@
       <c r="M121"/>
     </row>
     <row r="122" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B122" s="99">
+      <c r="B122" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>30</v>
       </c>
@@ -13633,18 +13579,18 @@
       <c r="E122" s="26" t="s">
         <v>679</v>
       </c>
-      <c r="F122" s="102">
-        <v>0</v>
-      </c>
-      <c r="G122" s="102">
-        <v>0</v>
-      </c>
-      <c r="H122" s="103" t="str">
+      <c r="F122" s="60">
+        <v>0</v>
+      </c>
+      <c r="G122" s="60">
+        <v>0</v>
+      </c>
+      <c r="H122" s="46" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I122" s="104" cm="1">
+      <c r="I122" s="34" cm="1">
         <f t="array" ref="I122" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
@@ -15561,11 +15507,11 @@
       </c>
     </row>
     <row r="172" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B172" s="99">
+      <c r="B172" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>21</v>
       </c>
-      <c r="C172" s="105" t="s">
+      <c r="C172" s="7" t="s">
         <v>677</v>
       </c>
       <c r="D172" s="28" t="s">
@@ -15592,7 +15538,7 @@
       <c r="K172" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="L172" s="106" t="s">
+      <c r="L172" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M172" s="27">
@@ -15604,17 +15550,17 @@
       <c r="O172" s="27">
         <v>1</v>
       </c>
-      <c r="P172" s="107" t="str">
+      <c r="P172" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="173" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B173" s="99">
+      <c r="B173" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>22</v>
       </c>
-      <c r="C173" s="105" t="s">
+      <c r="C173" s="7" t="s">
         <v>677</v>
       </c>
       <c r="D173" s="28" t="s">
@@ -15641,7 +15587,7 @@
       <c r="K173" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="L173" s="106" t="s">
+      <c r="L173" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M173" s="27">
@@ -15653,7 +15599,7 @@
       <c r="O173" s="27">
         <v>1</v>
       </c>
-      <c r="P173" s="107" t="str">
+      <c r="P173" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
@@ -18492,7 +18438,7 @@
       <c r="J249" s="65"/>
     </row>
     <row r="250" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B250" s="108">
+      <c r="B250" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>37</v>
       </c>
@@ -18514,7 +18460,7 @@
       <c r="H250" s="81" t="s">
         <v>225</v>
       </c>
-      <c r="I250" s="109" t="s">
+      <c r="I250" s="48" t="s">
         <v>191</v>
       </c>
       <c r="J250" s="65"/>

</xml_diff>

<commit_message>
formatting updates new AQ endpoints
changes to align new AQ endpoint csv
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0C96B0-6103-47AA-845A-F7651427D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C48D72-239D-4125-BA7B-544C02C3AE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3359,7 +3359,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3606,21 +3606,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9937,9 +9922,9 @@
   </sheetPr>
   <dimension ref="A1:U401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H49" sqref="H49"/>
+      <selection pane="topRight" activeCell="H223" sqref="H223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14793,7 +14778,7 @@
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B154" s="92">
+      <c r="B154" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>3</v>
       </c>
@@ -14824,7 +14809,7 @@
       <c r="K154" s="28" t="s">
         <v>718</v>
       </c>
-      <c r="L154" s="93" t="s">
+      <c r="L154" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M154" s="27">
@@ -14836,13 +14821,13 @@
       <c r="O154" s="27">
         <v>1</v>
       </c>
-      <c r="P154" s="94" t="str">
+      <c r="P154" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B155" s="92">
+      <c r="B155" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>4</v>
       </c>
@@ -14885,13 +14870,13 @@
       <c r="O155" s="27">
         <v>0.06</v>
       </c>
-      <c r="P155" s="94">
+      <c r="P155" s="33">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>2010</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B156" s="92">
+      <c r="B156" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>5</v>
       </c>
@@ -14934,13 +14919,13 @@
       <c r="O156" s="27">
         <v>1</v>
       </c>
-      <c r="P156" s="94">
+      <c r="P156" s="33">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>2010</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B157" s="92">
+      <c r="B157" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>6</v>
       </c>
@@ -14971,7 +14956,7 @@
       <c r="K157" s="28" t="s">
         <v>718</v>
       </c>
-      <c r="L157" s="93" t="s">
+      <c r="L157" s="28" t="s">
         <v>91</v>
       </c>
       <c r="M157" s="27">
@@ -14983,13 +14968,13 @@
       <c r="O157" s="27">
         <v>1</v>
       </c>
-      <c r="P157" s="94" t="str">
+      <c r="P157" s="33" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B158" s="92">
+      <c r="B158" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>7</v>
       </c>
@@ -15032,7 +15017,7 @@
       <c r="O158" s="27">
         <v>0.06</v>
       </c>
-      <c r="P158" s="94">
+      <c r="P158" s="33">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>2010</v>
       </c>
@@ -16998,7 +16983,7 @@
       </c>
     </row>
     <row r="199" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B199" s="92">
+      <c r="B199" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>48</v>
       </c>
@@ -17041,7 +17026,7 @@
       <c r="O199" s="27">
         <v>0.06</v>
       </c>
-      <c r="P199" s="94">
+      <c r="P199" s="33">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>2010</v>
       </c>
@@ -17587,7 +17572,7 @@
       </c>
     </row>
     <row r="211" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B211" s="92">
+      <c r="B211" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>60</v>
       </c>
@@ -17630,7 +17615,7 @@
       <c r="O211" s="27">
         <v>0.06</v>
       </c>
-      <c r="P211" s="94">
+      <c r="P211" s="33">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>2010</v>
       </c>
@@ -17889,7 +17874,7 @@
       <c r="S220" s="5"/>
     </row>
     <row r="221" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B221" s="95">
+      <c r="B221" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
@@ -17922,7 +17907,7 @@
       <c r="S221" s="5"/>
     </row>
     <row r="222" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B222" s="95">
+      <c r="B222" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
@@ -17955,7 +17940,7 @@
       <c r="S222" s="5"/>
     </row>
     <row r="223" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B223" s="95">
+      <c r="B223" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>3</v>
       </c>
@@ -17988,7 +17973,7 @@
       <c r="S223" s="5"/>
     </row>
     <row r="224" spans="1:21" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B224" s="95">
+      <c r="B224" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>4</v>
       </c>
@@ -18021,7 +18006,7 @@
       <c r="S224" s="5"/>
     </row>
     <row r="225" spans="2:19" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B225" s="95">
+      <c r="B225" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>5</v>
       </c>
@@ -18343,7 +18328,7 @@
       <c r="S234"/>
     </row>
     <row r="235" spans="2:19" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B235" s="95">
+      <c r="B235" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>15</v>
       </c>
@@ -18376,7 +18361,7 @@
       <c r="S235"/>
     </row>
     <row r="236" spans="2:19" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="B236" s="95">
+      <c r="B236" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>16</v>
       </c>
@@ -18409,7 +18394,7 @@
       <c r="S236"/>
     </row>
     <row r="237" spans="2:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="B237" s="95">
+      <c r="B237" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>17</v>
       </c>
@@ -18428,7 +18413,7 @@
       <c r="G237" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="H237" s="96">
+      <c r="H237" s="81">
         <v>2015</v>
       </c>
       <c r="I237" s="48" t="s">
@@ -18440,7 +18425,7 @@
       <c r="S237"/>
     </row>
     <row r="238" spans="2:19" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B238" s="95">
+      <c r="B238" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>18</v>
       </c>
@@ -18459,7 +18444,7 @@
       <c r="G238" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="H238" s="96">
+      <c r="H238" s="81">
         <v>2015</v>
       </c>
       <c r="I238" s="48" t="s">
@@ -18471,7 +18456,7 @@
       <c r="S238"/>
     </row>
     <row r="239" spans="2:19" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B239" s="95">
+      <c r="B239" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>19</v>
       </c>
@@ -18490,7 +18475,7 @@
       <c r="G239" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="H239" s="96">
+      <c r="H239" s="81">
         <v>2015</v>
       </c>
       <c r="I239" s="48" t="s">
@@ -18825,7 +18810,7 @@
       <c r="J250" s="65"/>
     </row>
     <row r="251" spans="2:19" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B251" s="95">
+      <c r="B251" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>31</v>
       </c>
@@ -18963,7 +18948,7 @@
       <c r="J255" s="65"/>
     </row>
     <row r="256" spans="2:19" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B256" s="95">
+      <c r="B256" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>36</v>
       </c>
@@ -18982,7 +18967,7 @@
       <c r="G256" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="H256" s="96">
+      <c r="H256" s="81">
         <v>2015</v>
       </c>
       <c r="I256" s="48" t="s">
@@ -19331,7 +19316,7 @@
       <c r="J268" s="65"/>
     </row>
     <row r="269" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B269" s="95">
+      <c r="B269" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>49</v>
       </c>
@@ -19359,7 +19344,7 @@
       <c r="J269" s="65"/>
     </row>
     <row r="270" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B270" s="95">
+      <c r="B270" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>50</v>
       </c>
@@ -19387,7 +19372,7 @@
       <c r="J270" s="65"/>
     </row>
     <row r="271" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B271" s="95">
+      <c r="B271" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Commented lines in some functions
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D821F022-418D-4723-901F-7625AD07C2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796C10B5-D7B8-480B-A443-6343A6B34501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -2612,7 +2612,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2822,18 +2822,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7596,9 +7584,9 @@
   </sheetPr>
   <dimension ref="A1:U285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C246" sqref="C246"/>
+      <selection pane="topRight" activeCell="D220" sqref="D220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15643,7 +15631,7 @@
       <c r="J244" s="55"/>
     </row>
     <row r="245" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B245" s="77">
+      <c r="B245" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>26</v>
       </c>
@@ -15656,16 +15644,16 @@
       <c r="E245" s="70" t="s">
         <v>505</v>
       </c>
-      <c r="F245" s="78">
+      <c r="F245" s="70">
         <v>0</v>
       </c>
-      <c r="G245" s="78">
+      <c r="G245" s="70">
         <v>0</v>
       </c>
-      <c r="H245" s="79" t="s">
+      <c r="H245" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="I245" s="80" t="s">
+      <c r="I245" s="38" t="s">
         <v>182</v>
       </c>
       <c r="J245" s="55"/>

</xml_diff>

<commit_message>
Second National Level Revision
Updated scaled impacts for: National Forestry, State Forestry, National Extreme Temp.
Updated scalars for: National Forestry (deleted), State Forestry (deleted), National AQ, State AQ, National Wildfire, State Wildfire, National SW Dust, State SW Dust, National CIL Crime, Outdoor Recreation.
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/FrEDI_config.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E01E1E9-6900-4FD4-956B-3E86C9FB853B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFFDAF3-1EFA-4ECF-9B44-9DF5DEB9D763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="739">
   <si>
     <t>CanESM2</t>
   </si>
@@ -9922,9 +9922,9 @@
   </sheetPr>
   <dimension ref="A1:U401"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J213" sqref="J213"/>
+      <selection pane="topRight" activeCell="K120" sqref="K120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13378,9 +13378,7 @@
       <c r="G114" s="60">
         <v>1</v>
       </c>
-      <c r="H114" s="46" t="s">
-        <v>659</v>
-      </c>
+      <c r="H114" s="46"/>
       <c r="I114" s="34" cm="1">
         <f t="array" ref="I114" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
@@ -13410,9 +13408,7 @@
       <c r="G115" s="60">
         <v>0</v>
       </c>
-      <c r="H115" s="46" t="s">
-        <v>660</v>
-      </c>
+      <c r="H115" s="46"/>
       <c r="I115" s="34" cm="1">
         <f t="array" ref="I115" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
         <v>1</v>
@@ -15521,7 +15517,7 @@
         <v>90</v>
       </c>
       <c r="J173" s="28" t="s">
-        <v>738</v>
+        <v>90</v>
       </c>
       <c r="K173" s="28" t="s">
         <v>91</v>
@@ -19323,7 +19319,7 @@
       <c r="I276" s="48"/>
       <c r="J276" s="65"/>
     </row>
-    <row r="277" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:21" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B277" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>57</v>
@@ -21667,7 +21663,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <f xml:space="preserve"> ROW( testDev[[#This Row],[row_id]] ) - ROW(testDev[[#Headers],[row_id]] )</f>
         <v>6</v>

</xml_diff>